<commit_message>
AutoDS Tests validation OK + analyse sensibilité ordre des données
</commit_message>
<xml_diff>
--- a/AutoDS/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
+++ b/AutoDS/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\jpm-sandbox\perso\AutoDS\refout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CFD30B-2EB1-4DCF-8B3D-02F9A60E1B17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E776F50-DB4E-4E3E-97DE-E1F91C4AC531}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="96" yWindow="48" windowWidth="19620" windowHeight="13176" tabRatio="220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BC3BDE-F4BA-4050-8B7E-D00DA3DA3E40}">
   <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,13 +1910,76 @@
         <v>62</v>
       </c>
       <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="2">
+        <v>43674.877928240741</v>
+      </c>
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="F17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="2">
-        <v>43648.778692129628</v>
+      <c r="I17">
+        <v>217</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>2318.1190000000001</v>
+      </c>
+      <c r="L17">
+        <v>0.14708280000000001</v>
+      </c>
+      <c r="M17">
+        <v>0.56151450000000003</v>
+      </c>
+      <c r="N17">
+        <v>0.7</v>
+      </c>
+      <c r="O17">
+        <v>0.6</v>
+      </c>
+      <c r="P17">
+        <v>175.24680000000001</v>
+      </c>
+      <c r="Q17">
+        <v>165.1386</v>
+      </c>
+      <c r="R17">
+        <v>185.97370000000001</v>
+      </c>
+      <c r="S17" s="3">
+        <v>3.0148089999999999E-2</v>
+      </c>
+      <c r="T17">
+        <v>0.10813</v>
+      </c>
+      <c r="U17">
+        <v>8.4577399999999997E-2</v>
+      </c>
+      <c r="V17">
+        <v>0.13824139999999999</v>
+      </c>
+      <c r="W17">
+        <v>0.1249212</v>
+      </c>
+      <c r="X17">
+        <v>0.34123829999999999</v>
+      </c>
+      <c r="Y17">
+        <v>0.30303289999999999</v>
+      </c>
+      <c r="Z17">
+        <v>0.3842604</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>6.0296170000000003E-2</v>
+      </c>
+      <c r="AB17">
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
@@ -1936,10 +1999,10 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="G18" s="2">
-        <v>43648.695138888892</v>
+        <v>43674.878622685188</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -1948,60 +2011,60 @@
         <v>217</v>
       </c>
       <c r="J18">
-        <v>9.4890139999999992</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>2327.6080000000002</v>
-      </c>
-      <c r="L18" s="3">
-        <v>3.3778610000000001E-2</v>
-      </c>
-      <c r="M18" s="3">
-        <v>2.1573459999999999E-2</v>
+        <v>2318.1190000000001</v>
+      </c>
+      <c r="L18">
+        <v>0.14708280000000001</v>
+      </c>
+      <c r="M18">
+        <v>0.56151450000000003</v>
       </c>
       <c r="N18">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="O18">
-        <v>0.05</v>
+        <v>0.6</v>
       </c>
       <c r="P18">
-        <v>146.255</v>
+        <v>175.24680000000001</v>
       </c>
       <c r="Q18">
-        <v>133.4556</v>
+        <v>165.1386</v>
       </c>
       <c r="R18">
-        <v>160.28190000000001</v>
+        <v>185.97370000000001</v>
       </c>
       <c r="S18" s="3">
-        <v>4.6488710000000003E-2</v>
+        <v>3.0148089999999999E-2</v>
       </c>
       <c r="T18">
-        <v>0.15524769999999999</v>
+        <v>0.10813</v>
       </c>
       <c r="U18">
-        <v>0.1171735</v>
+        <v>8.4577399999999997E-2</v>
       </c>
       <c r="V18">
-        <v>0.2056935</v>
+        <v>0.13824139999999999</v>
       </c>
       <c r="W18">
-        <v>0.1435775</v>
+        <v>0.1249212</v>
       </c>
       <c r="X18">
-        <v>0.23767250000000001</v>
+        <v>0.34123829999999999</v>
       </c>
       <c r="Y18">
-        <v>0.19795189999999999</v>
+        <v>0.30303289999999999</v>
       </c>
       <c r="Z18">
-        <v>0.28536339999999999</v>
+        <v>0.3842604</v>
       </c>
       <c r="AA18" s="3">
-        <v>9.297743E-2</v>
-      </c>
-      <c r="AB18" s="23">
+        <v>6.0296170000000003E-2</v>
+      </c>
+      <c r="AB18">
         <v>215</v>
       </c>
     </row>
@@ -2022,10 +2085,10 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G19" s="2">
-        <v>43648.695162037038</v>
+        <v>43674.878668981481</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -2033,61 +2096,61 @@
       <c r="I19">
         <v>217</v>
       </c>
-      <c r="J19" s="3">
-        <v>2.0019530000000001E-2</v>
+      <c r="J19">
+        <v>9.4890139999999992</v>
       </c>
       <c r="K19">
-        <v>2318.1390000000001</v>
+        <v>2327.6080000000002</v>
       </c>
       <c r="L19" s="3">
-        <v>2.5966110000000001E-2</v>
-      </c>
-      <c r="M19">
-        <v>0.19065989999999999</v>
+        <v>3.3778610000000001E-2</v>
+      </c>
+      <c r="M19" s="3">
+        <v>2.1573459999999999E-2</v>
       </c>
       <c r="N19">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O19">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="P19">
-        <v>159.67529999999999</v>
+        <v>146.255</v>
       </c>
       <c r="Q19">
-        <v>153.85550000000001</v>
+        <v>133.4556</v>
       </c>
       <c r="R19">
-        <v>165.71530000000001</v>
+        <v>160.28190000000001</v>
       </c>
       <c r="S19" s="3">
-        <v>1.883862E-2</v>
+        <v>4.6488710000000003E-2</v>
       </c>
       <c r="T19">
-        <v>0.130248</v>
+        <v>0.15524769999999999</v>
       </c>
       <c r="U19">
-        <v>0.1036734</v>
+        <v>0.1171735</v>
       </c>
       <c r="V19">
-        <v>0.16363449999999999</v>
+        <v>0.2056935</v>
       </c>
       <c r="W19">
-        <v>0.115712</v>
+        <v>0.1435775</v>
       </c>
       <c r="X19">
-        <v>0.28329110000000002</v>
+        <v>0.23767250000000001</v>
       </c>
       <c r="Y19">
-        <v>0.26302189999999998</v>
+        <v>0.19795189999999999</v>
       </c>
       <c r="Z19">
-        <v>0.30512230000000001</v>
+        <v>0.28536339999999999</v>
       </c>
       <c r="AA19" s="3">
-        <v>3.7677240000000001E-2</v>
-      </c>
-      <c r="AB19" s="23">
+        <v>9.297743E-2</v>
+      </c>
+      <c r="AB19">
         <v>215</v>
       </c>
     </row>
@@ -2108,73 +2171,73 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G20" s="2">
-        <v>43648.695173611108</v>
+        <v>43674.878692129627</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20">
         <v>217</v>
       </c>
-      <c r="J20">
-        <v>0.60717770000000004</v>
+      <c r="J20" s="3">
+        <v>2.0019530000000001E-2</v>
       </c>
       <c r="K20">
-        <v>2318.7260000000001</v>
-      </c>
-      <c r="L20">
-        <v>0.1377766</v>
+        <v>2318.1390000000001</v>
+      </c>
+      <c r="L20" s="3">
+        <v>2.5966110000000001E-2</v>
       </c>
       <c r="M20">
-        <v>0.37742910000000002</v>
+        <v>0.19065989999999999</v>
       </c>
       <c r="N20">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="O20">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="P20">
-        <v>170.41839999999999</v>
+        <v>159.67529999999999</v>
       </c>
       <c r="Q20">
-        <v>114.8882</v>
+        <v>153.85550000000001</v>
       </c>
       <c r="R20">
-        <v>252.7886</v>
-      </c>
-      <c r="S20">
-        <v>0.20205590000000001</v>
+        <v>165.71530000000001</v>
+      </c>
+      <c r="S20" s="3">
+        <v>1.883862E-2</v>
       </c>
       <c r="T20">
-        <v>0.1143441</v>
-      </c>
-      <c r="U20" s="3">
-        <v>5.1812080000000003E-2</v>
+        <v>0.130248</v>
+      </c>
+      <c r="U20">
+        <v>0.1036734</v>
       </c>
       <c r="V20">
-        <v>0.25234600000000001</v>
+        <v>0.16363449999999999</v>
       </c>
       <c r="W20">
-        <v>0.41865970000000002</v>
+        <v>0.115712</v>
       </c>
       <c r="X20">
-        <v>0.32269350000000002</v>
+        <v>0.28329110000000002</v>
       </c>
       <c r="Y20">
-        <v>0.14991670000000001</v>
+        <v>0.26302189999999998</v>
       </c>
       <c r="Z20">
-        <v>0.69459329999999997</v>
-      </c>
-      <c r="AA20">
-        <v>0.40411170000000002</v>
-      </c>
-      <c r="AB20" s="23">
-        <v>214</v>
+        <v>0.30512230000000001</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>3.7677240000000001E-2</v>
+      </c>
+      <c r="AB20">
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
@@ -2191,76 +2254,76 @@
         <v>62</v>
       </c>
       <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="2">
+        <v>43674.878877314812</v>
+      </c>
+      <c r="H21">
         <v>3</v>
-      </c>
-      <c r="F21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="2">
-        <v>43648.695115740738</v>
-      </c>
-      <c r="H21">
-        <v>2</v>
       </c>
       <c r="I21">
         <v>217</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>0.60717770000000004</v>
       </c>
       <c r="K21">
-        <v>2318.1190000000001</v>
+        <v>2318.7260000000001</v>
       </c>
       <c r="L21">
-        <v>0.14708280000000001</v>
+        <v>0.1377766</v>
       </c>
       <c r="M21">
-        <v>0.56151450000000003</v>
+        <v>0.37742910000000002</v>
       </c>
       <c r="N21">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="O21">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="P21">
-        <v>175.24680000000001</v>
+        <v>170.41839999999999</v>
       </c>
       <c r="Q21">
-        <v>165.1386</v>
+        <v>114.8882</v>
       </c>
       <c r="R21">
-        <v>185.97370000000001</v>
-      </c>
-      <c r="S21" s="3">
-        <v>3.0148089999999999E-2</v>
+        <v>252.7886</v>
+      </c>
+      <c r="S21">
+        <v>0.20205590000000001</v>
       </c>
       <c r="T21">
-        <v>0.10813</v>
-      </c>
-      <c r="U21">
-        <v>8.4577399999999997E-2</v>
+        <v>0.1143441</v>
+      </c>
+      <c r="U21" s="3">
+        <v>5.1812080000000003E-2</v>
       </c>
       <c r="V21">
-        <v>0.13824139999999999</v>
+        <v>0.25234600000000001</v>
       </c>
       <c r="W21">
-        <v>0.1249212</v>
+        <v>0.41865970000000002</v>
       </c>
       <c r="X21">
-        <v>0.34123829999999999</v>
+        <v>0.32269350000000002</v>
       </c>
       <c r="Y21">
-        <v>0.30303289999999999</v>
+        <v>0.14991670000000001</v>
       </c>
       <c r="Z21">
-        <v>0.3842604</v>
-      </c>
-      <c r="AA21" s="3">
-        <v>6.0296170000000003E-2</v>
-      </c>
-      <c r="AB21" s="23">
-        <v>215</v>
+        <v>0.69459329999999997</v>
+      </c>
+      <c r="AA21">
+        <v>0.40411170000000002</v>
+      </c>
+      <c r="AB21">
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.3">
@@ -2283,7 +2346,7 @@
         <v>35</v>
       </c>
       <c r="G22" s="2">
-        <v>43648.672037037039</v>
+        <v>43674.886631944442</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -2345,7 +2408,7 @@
       <c r="AA22" s="3">
         <v>6.029524E-2</v>
       </c>
-      <c r="AB22" s="23">
+      <c r="AB22">
         <v>215</v>
       </c>
     </row>
@@ -2369,7 +2432,7 @@
         <v>36</v>
       </c>
       <c r="G23" s="2">
-        <v>43648.672060185185</v>
+        <v>43674.88685185185</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -2431,7 +2494,7 @@
       <c r="AA23" s="3">
         <v>6.029524E-2</v>
       </c>
-      <c r="AB23" s="23">
+      <c r="AB23">
         <v>215</v>
       </c>
     </row>
@@ -2455,7 +2518,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="2">
-        <v>43648.672083333331</v>
+        <v>43674.886793981481</v>
       </c>
       <c r="H24">
         <v>3</v>
@@ -2517,7 +2580,7 @@
       <c r="AA24">
         <v>0.20112250000000001</v>
       </c>
-      <c r="AB24" s="23">
+      <c r="AB24">
         <v>214</v>
       </c>
     </row>
@@ -2541,7 +2604,7 @@
         <v>37</v>
       </c>
       <c r="G25" s="2">
-        <v>43648.672106481485</v>
+        <v>43674.886747685188</v>
       </c>
       <c r="H25">
         <v>2</v>
@@ -2603,7 +2666,7 @@
       <c r="AA25" s="3">
         <v>3.8218509999999997E-2</v>
       </c>
-      <c r="AB25" s="23">
+      <c r="AB25">
         <v>215</v>
       </c>
     </row>
@@ -2627,7 +2690,7 @@
         <v>34</v>
       </c>
       <c r="G26" s="2">
-        <v>43648.672129629631</v>
+        <v>43674.886701388888</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -2689,7 +2752,7 @@
       <c r="AA26">
         <v>0.40410849999999998</v>
       </c>
-      <c r="AB26" s="23">
+      <c r="AB26">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoDS Rapports HTML/Excel quasi-OK (reste quel Chi2P, nan HTML, seuils couleur DCV) + troncatures à gérer
</commit_message>
<xml_diff>
--- a/AutoDS/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
+++ b/AutoDS/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\jpm-sandbox\perso\AutoDS\refout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E776F50-DB4E-4E3E-97DE-E1F91C4AC531}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16D7F96-2148-4E2B-9688-B95CF02BDFA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="96" yWindow="48" windowWidth="19620" windowHeight="13176" tabRatio="220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,9 +205,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Sample</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>P DF</t>
+  </si>
+  <si>
+    <t>Periods</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:AB26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,13 +714,13 @@
         <v>57</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>59</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>20</v>
@@ -792,7 +792,7 @@
         <v>56</v>
       </c>
       <c r="AB1" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -803,10 +803,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -889,10 +889,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -975,10 +975,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1061,10 +1061,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1147,10 +1147,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1170,10 +1170,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1256,10 +1256,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1342,10 +1342,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1428,10 +1428,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1514,10 +1514,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -1537,10 +1537,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1623,10 +1623,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1709,10 +1709,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1795,10 +1795,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -1881,10 +1881,10 @@
         <v>11</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1904,10 +1904,10 @@
         <v>11</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1990,10 +1990,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -2076,10 +2076,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -2162,10 +2162,10 @@
         <v>11</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -2248,10 +2248,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -2334,10 +2334,10 @@
         <v>11</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -2420,10 +2420,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -2506,10 +2506,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -2592,10 +2592,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -2678,10 +2678,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -2774,7 +2774,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AutoDS Finalisation support spec tranches dist pour fitting ET discrétisation + npon régression + préparation nouveaux cas tests
</commit_message>
<xml_diff>
--- a/AutoDS/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
+++ b/AutoDS/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\jpm-sandbox\perso\AutoDS\refout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33910057-2D42-457A-8607-AA3A52B7A690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F2739D-E112-4514-9878-56320C612236}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="48" windowWidth="19620" windowHeight="9564" tabRatio="220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="96" yWindow="48" windowWidth="19620" windowHeight="9564" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultats" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="90">
   <si>
     <t>TURMER</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Periods</t>
   </si>
   <si>
-    <t>DistCuts</t>
-  </si>
-  <si>
     <t>RTrunc</t>
   </si>
   <si>
@@ -275,19 +272,34 @@
     <t>Half-Norm Cos TGD</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>40,90,140,190,240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tronc gauche et droite (dists = ?) et N? tranches </t>
-  </si>
-  <si>
-    <t>Hazard Cos TGDN</t>
-  </si>
-  <si>
-    <t>Hazard Cos TGDInt</t>
+    <t>FitDistCuts</t>
+  </si>
+  <si>
+    <t>Hazard Cos TGDEstInt</t>
+  </si>
+  <si>
+    <t>90,140,190</t>
+  </si>
+  <si>
+    <t>Hazard Cos TGDFitCls</t>
+  </si>
+  <si>
+    <t>Hazard SimPolyFitInt</t>
+  </si>
+  <si>
+    <t>Hazard SimPoly TGDFitInt</t>
+  </si>
+  <si>
+    <t>Hazard Cos TGDDiscrCls</t>
+  </si>
+  <si>
+    <t>Hazard Cos TGDDiscrInt</t>
+  </si>
+  <si>
+    <t>DiscrDistCuts</t>
+  </si>
+  <si>
+    <t>Hazard Cos TGDiscrCls</t>
   </si>
 </sst>
 </file>
@@ -297,7 +309,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,13 +326,6 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -382,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -414,9 +419,6 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="22" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -758,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BC3BDE-F4BA-4050-8B7E-D00DA3DA3E40}">
-  <dimension ref="A1:AF31"/>
+  <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,13 +772,14 @@
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" customWidth="1"/>
-    <col min="9" max="10" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" customWidth="1"/>
     <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.44140625" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="10" bestFit="1" customWidth="1"/>
@@ -810,15 +813,17 @@
         <v>21</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="K1" s="21" t="s">
         <v>22</v>
       </c>
@@ -1281,7 +1286,7 @@
       <c r="M7">
         <v>423</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="25">
         <f>O7-O10</f>
         <v>178.79500000000007</v>
       </c>
@@ -1368,7 +1373,7 @@
       <c r="M8">
         <v>423</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="25">
         <f>O8-O10</f>
         <v>178.79500000000007</v>
       </c>
@@ -1455,7 +1460,7 @@
       <c r="M9">
         <v>423</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="25">
         <f>O9-O10</f>
         <v>168.65500000000065</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="10" spans="1:32" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1527,80 +1532,80 @@
       <c r="D10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="28">
-        <v>1</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="28">
+      <c r="E10" s="25">
+        <v>1</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="25">
         <v>300</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="26">
         <v>43737.668692129628</v>
       </c>
-      <c r="L10" s="28">
-        <v>1</v>
-      </c>
-      <c r="M10" s="28">
+      <c r="L10" s="25">
+        <v>1</v>
+      </c>
+      <c r="M10" s="25">
         <v>415</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="25">
         <f>O10-O10</f>
         <v>0</v>
       </c>
-      <c r="O10" s="28">
+      <c r="O10" s="25">
         <v>4479.3289999999997</v>
       </c>
-      <c r="P10" s="28">
+      <c r="P10" s="25">
         <v>0.3184978</v>
       </c>
-      <c r="Q10" s="28">
+      <c r="Q10" s="25">
         <v>0.89928859999999999</v>
       </c>
-      <c r="R10" s="28">
+      <c r="R10" s="25">
         <v>0.8</v>
       </c>
-      <c r="S10" s="28">
+      <c r="S10" s="25">
         <v>0.8</v>
       </c>
-      <c r="T10" s="28">
+      <c r="T10" s="25">
         <v>118.8552</v>
       </c>
-      <c r="U10" s="28">
+      <c r="U10" s="25">
         <v>113.4011</v>
       </c>
-      <c r="V10" s="28">
+      <c r="V10" s="25">
         <v>124.57170000000001</v>
       </c>
-      <c r="W10" s="30">
+      <c r="W10" s="27">
         <v>2.3900879999999999E-2</v>
       </c>
-      <c r="X10" s="28">
+      <c r="X10" s="25">
         <v>0.4495709</v>
       </c>
-      <c r="Y10" s="28">
+      <c r="Y10" s="25">
         <v>0.38879730000000001</v>
       </c>
-      <c r="Z10" s="28">
+      <c r="Z10" s="25">
         <v>0.51984419999999998</v>
       </c>
-      <c r="AA10" s="30">
+      <c r="AA10" s="27">
         <v>7.3869409999999996E-2</v>
       </c>
-      <c r="AB10" s="28">
+      <c r="AB10" s="25">
         <v>0.15696189999999999</v>
       </c>
-      <c r="AC10" s="28">
+      <c r="AC10" s="25">
         <v>0.14289250000000001</v>
       </c>
-      <c r="AD10" s="28">
+      <c r="AD10" s="25">
         <v>0.1724166</v>
       </c>
-      <c r="AE10" s="30">
+      <c r="AE10" s="27">
         <v>4.7801759999999999E-2</v>
       </c>
-      <c r="AF10" s="28">
+      <c r="AF10" s="25">
         <v>414</v>
       </c>
     </row>
@@ -1632,7 +1637,7 @@
       <c r="M11">
         <v>423</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="25">
         <f>O11-O10</f>
         <v>235.15500000000065</v>
       </c>
@@ -1992,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G16">
         <v>30</v>
@@ -2209,7 +2214,8 @@
         <v>217</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <f>O19-O22</f>
+        <v>1777.3537000000001</v>
       </c>
       <c r="O19">
         <v>2318.1190000000001</v>
@@ -2295,7 +2301,8 @@
         <v>217</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <f>O20-O22</f>
+        <v>1777.3537000000001</v>
       </c>
       <c r="O20">
         <v>2318.1190000000001</v>
@@ -2352,7 +2359,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:32" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -2365,85 +2372,86 @@
       <c r="D21" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="28">
-        <v>1</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="28">
+      <c r="E21" s="25">
+        <v>1</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="25">
         <v>40</v>
       </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29">
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26">
         <v>43737.674988425926</v>
       </c>
-      <c r="L21" s="28">
-        <v>2</v>
-      </c>
-      <c r="M21" s="28">
+      <c r="L21" s="25">
+        <v>2</v>
+      </c>
+      <c r="M21" s="25">
         <v>215</v>
       </c>
-      <c r="N21" s="28">
-        <v>0</v>
-      </c>
-      <c r="O21" s="28">
+      <c r="N21">
+        <f>O21-O22</f>
+        <v>1729.3157000000001</v>
+      </c>
+      <c r="O21" s="25">
         <v>2270.0810000000001</v>
       </c>
-      <c r="P21" s="28">
+      <c r="P21" s="25">
         <v>0.69110099999999997</v>
       </c>
-      <c r="Q21" s="28">
+      <c r="Q21" s="25">
         <v>0.92968229999999996</v>
       </c>
-      <c r="R21" s="28">
+      <c r="R21" s="25">
         <v>0.9</v>
       </c>
-      <c r="S21" s="28">
+      <c r="S21" s="25">
         <v>0.9</v>
       </c>
-      <c r="T21" s="28">
+      <c r="T21" s="25">
         <v>166.21420000000001</v>
       </c>
-      <c r="U21" s="28">
+      <c r="U21" s="25">
         <v>155.69970000000001</v>
       </c>
-      <c r="V21" s="28">
+      <c r="V21" s="25">
         <v>177.43879999999999</v>
       </c>
-      <c r="W21" s="30">
+      <c r="W21" s="27">
         <v>3.3161290000000003E-2</v>
       </c>
-      <c r="X21" s="28">
+      <c r="X21" s="25">
         <v>0.1190937</v>
       </c>
-      <c r="Y21" s="30">
+      <c r="Y21" s="27">
         <v>9.2797210000000005E-2</v>
       </c>
-      <c r="Z21" s="28">
+      <c r="Z21" s="25">
         <v>0.15284200000000001</v>
       </c>
-      <c r="AA21" s="28">
+      <c r="AA21" s="25">
         <v>0.12695770000000001</v>
       </c>
-      <c r="AB21" s="28">
+      <c r="AB21" s="25">
         <v>0.30696859999999998</v>
       </c>
-      <c r="AC21" s="28">
+      <c r="AC21" s="25">
         <v>0.26938889999999999</v>
       </c>
-      <c r="AD21" s="28">
+      <c r="AD21" s="25">
         <v>0.34979060000000001</v>
       </c>
-      <c r="AE21" s="30">
+      <c r="AE21" s="27">
         <v>6.6322569999999997E-2</v>
       </c>
-      <c r="AF21" s="28">
+      <c r="AF21" s="25">
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
@@ -2456,77 +2464,82 @@
       <c r="D22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
+      <c r="E22" s="25">
+        <v>2</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="25">
+        <v>40</v>
+      </c>
+      <c r="H22" s="25">
+        <v>240</v>
+      </c>
+      <c r="I22" s="26"/>
+      <c r="J22" s="25">
+        <v>4</v>
       </c>
       <c r="K22" s="2">
-        <v>43674.878668981481</v>
+        <v>43739.628611111111</v>
       </c>
       <c r="L22">
         <v>2</v>
       </c>
-      <c r="M22">
-        <v>217</v>
+      <c r="M22" s="25">
+        <v>210</v>
       </c>
       <c r="N22">
-        <v>9.4890139999999992</v>
+        <f t="shared" ref="N22" si="0">O22-O22</f>
+        <v>0</v>
       </c>
       <c r="O22">
-        <v>2327.6080000000002</v>
-      </c>
-      <c r="P22" s="3">
-        <v>3.3778610000000001E-2</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>2.1573459999999999E-2</v>
-      </c>
-      <c r="R22">
-        <v>0.1</v>
-      </c>
-      <c r="S22">
-        <v>0.05</v>
-      </c>
+        <v>540.76530000000002</v>
+      </c>
+      <c r="P22">
+        <v>0.34615800000000002</v>
+      </c>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
       <c r="T22">
-        <v>146.255</v>
+        <v>160.13</v>
       </c>
       <c r="U22">
-        <v>133.4556</v>
+        <v>147.26949999999999</v>
       </c>
       <c r="V22">
-        <v>160.28190000000001</v>
+        <v>174.11349999999999</v>
       </c>
       <c r="W22" s="3">
-        <v>4.6488710000000003E-2</v>
+        <v>4.2486370000000002E-2</v>
       </c>
       <c r="X22">
-        <v>0.15524769999999999</v>
-      </c>
-      <c r="Y22">
-        <v>0.1171735</v>
+        <v>0.12533159999999999</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>9.5713560000000003E-2</v>
       </c>
       <c r="Z22">
-        <v>0.2056935</v>
+        <v>0.16411490000000001</v>
       </c>
       <c r="AA22">
-        <v>0.1435775</v>
+        <v>0.13746410000000001</v>
       </c>
       <c r="AB22">
-        <v>0.23767250000000001</v>
+        <v>0.44516689999999998</v>
       </c>
       <c r="AC22">
-        <v>0.19795189999999999</v>
+        <v>0.37661830000000002</v>
       </c>
       <c r="AD22">
-        <v>0.28536339999999999</v>
+        <v>0.52619210000000005</v>
       </c>
       <c r="AE22" s="3">
-        <v>9.297743E-2</v>
+        <v>8.497275E-2</v>
       </c>
       <c r="AF22">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.3">
@@ -2546,10 +2559,10 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="K23" s="2">
-        <v>43674.878692129627</v>
+        <v>43674.878668981481</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -2557,59 +2570,60 @@
       <c r="M23">
         <v>217</v>
       </c>
-      <c r="N23" s="3">
-        <v>2.0019530000000001E-2</v>
+      <c r="N23">
+        <f>O23-O22</f>
+        <v>1786.8427000000001</v>
       </c>
       <c r="O23">
-        <v>2318.1390000000001</v>
+        <v>2327.6080000000002</v>
       </c>
       <c r="P23" s="3">
-        <v>2.5966110000000001E-2</v>
-      </c>
-      <c r="Q23">
-        <v>0.19065989999999999</v>
+        <v>3.3778610000000001E-2</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>2.1573459999999999E-2</v>
       </c>
       <c r="R23">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S23">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="T23">
-        <v>159.67529999999999</v>
+        <v>146.255</v>
       </c>
       <c r="U23">
-        <v>153.85550000000001</v>
+        <v>133.4556</v>
       </c>
       <c r="V23">
-        <v>165.71530000000001</v>
+        <v>160.28190000000001</v>
       </c>
       <c r="W23" s="3">
-        <v>1.883862E-2</v>
+        <v>4.6488710000000003E-2</v>
       </c>
       <c r="X23">
-        <v>0.130248</v>
+        <v>0.15524769999999999</v>
       </c>
       <c r="Y23">
-        <v>0.1036734</v>
+        <v>0.1171735</v>
       </c>
       <c r="Z23">
-        <v>0.16363449999999999</v>
+        <v>0.2056935</v>
       </c>
       <c r="AA23">
-        <v>0.115712</v>
+        <v>0.1435775</v>
       </c>
       <c r="AB23">
-        <v>0.28329110000000002</v>
+        <v>0.23767250000000001</v>
       </c>
       <c r="AC23">
-        <v>0.26302189999999998</v>
+        <v>0.19795189999999999</v>
       </c>
       <c r="AD23">
-        <v>0.30512230000000001</v>
+        <v>0.28536339999999999</v>
       </c>
       <c r="AE23" s="3">
-        <v>3.7677240000000001E-2</v>
+        <v>9.297743E-2</v>
       </c>
       <c r="AF23">
         <v>215</v>
@@ -2632,199 +2646,251 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K24" s="2">
-        <v>43674.878877314812</v>
+        <v>43674.878692129627</v>
       </c>
       <c r="L24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M24">
         <v>217</v>
       </c>
       <c r="N24">
-        <v>0.60717770000000004</v>
+        <f>O24-O22</f>
+        <v>1777.3737000000001</v>
       </c>
       <c r="O24">
-        <v>2318.7260000000001</v>
-      </c>
-      <c r="P24">
-        <v>0.1377766</v>
+        <v>2318.1390000000001</v>
+      </c>
+      <c r="P24" s="3">
+        <v>2.5966110000000001E-2</v>
       </c>
       <c r="Q24">
-        <v>0.37742910000000002</v>
+        <v>0.19065989999999999</v>
       </c>
       <c r="R24">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="S24">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="T24">
-        <v>170.41839999999999</v>
+        <v>159.67529999999999</v>
       </c>
       <c r="U24">
-        <v>114.8882</v>
+        <v>153.85550000000001</v>
       </c>
       <c r="V24">
-        <v>252.7886</v>
-      </c>
-      <c r="W24">
-        <v>0.20205590000000001</v>
+        <v>165.71530000000001</v>
+      </c>
+      <c r="W24" s="3">
+        <v>1.883862E-2</v>
       </c>
       <c r="X24">
-        <v>0.1143441</v>
-      </c>
-      <c r="Y24" s="3">
-        <v>5.1812080000000003E-2</v>
+        <v>0.130248</v>
+      </c>
+      <c r="Y24">
+        <v>0.1036734</v>
       </c>
       <c r="Z24">
-        <v>0.25234600000000001</v>
+        <v>0.16363449999999999</v>
       </c>
       <c r="AA24">
-        <v>0.41865970000000002</v>
+        <v>0.115712</v>
       </c>
       <c r="AB24">
-        <v>0.32269350000000002</v>
+        <v>0.28329110000000002</v>
       </c>
       <c r="AC24">
-        <v>0.14991670000000001</v>
+        <v>0.26302189999999998</v>
       </c>
       <c r="AD24">
-        <v>0.69459329999999997</v>
-      </c>
-      <c r="AE24">
-        <v>0.40411170000000002</v>
+        <v>0.30512230000000001</v>
+      </c>
+      <c r="AE24" s="3">
+        <v>3.7677240000000001E-2</v>
       </c>
       <c r="AF24">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K25" s="2">
-        <v>43674.886631944442</v>
+        <v>43674.878877314812</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M25">
         <v>217</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25:N31" si="0">O25-O25</f>
-        <v>0</v>
+        <f>O25-O30</f>
+        <v>1777.9612000000002</v>
       </c>
       <c r="O25">
+        <v>2318.7260000000001</v>
+      </c>
+      <c r="P25">
+        <v>0.1377766</v>
+      </c>
+      <c r="Q25">
+        <v>0.37742910000000002</v>
+      </c>
+      <c r="R25">
+        <v>0.6</v>
+      </c>
+      <c r="S25">
+        <v>0.4</v>
+      </c>
+      <c r="T25">
+        <v>170.41839999999999</v>
+      </c>
+      <c r="U25">
+        <v>114.8882</v>
+      </c>
+      <c r="V25">
+        <v>252.7886</v>
+      </c>
+      <c r="W25">
+        <v>0.20205590000000001</v>
+      </c>
+      <c r="X25">
+        <v>0.1143441</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>5.1812080000000003E-2</v>
+      </c>
+      <c r="Z25">
+        <v>0.25234600000000001</v>
+      </c>
+      <c r="AA25">
+        <v>0.41865970000000002</v>
+      </c>
+      <c r="AB25">
+        <v>0.32269350000000002</v>
+      </c>
+      <c r="AC25">
+        <v>0.14991670000000001</v>
+      </c>
+      <c r="AD25">
+        <v>0.69459329999999997</v>
+      </c>
+      <c r="AE25">
+        <v>0.40411170000000002</v>
+      </c>
+      <c r="AF25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="2">
+        <v>43674.886631944442</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>217</v>
+      </c>
+      <c r="N26">
+        <f>O26-O30</f>
+        <v>1777.3522000000003</v>
+      </c>
+      <c r="O26">
         <v>2318.1170000000002</v>
       </c>
-      <c r="P25">
+      <c r="P26">
         <v>0.14716180000000001</v>
       </c>
-      <c r="Q25">
+      <c r="Q26">
         <v>0.56517220000000001</v>
       </c>
-      <c r="R25">
+      <c r="R26">
         <v>0.7</v>
       </c>
-      <c r="S25">
+      <c r="S26">
         <v>0.6</v>
       </c>
-      <c r="T25">
+      <c r="T26">
         <v>175.25049999999999</v>
       </c>
-      <c r="U25">
+      <c r="U26">
         <v>165.1422</v>
       </c>
-      <c r="V25">
+      <c r="V26">
         <v>185.97749999999999</v>
       </c>
-      <c r="W25" s="3">
+      <c r="W26" s="3">
         <v>3.014762E-2</v>
       </c>
-      <c r="X25">
+      <c r="X26">
         <v>0.1081255</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Y26" s="3">
         <v>8.4573930000000005E-2</v>
       </c>
-      <c r="Z25">
+      <c r="Z26">
         <v>0.13823550000000001</v>
       </c>
-      <c r="AA25">
+      <c r="AA26">
         <v>0.1249208</v>
       </c>
-      <c r="AB25">
+      <c r="AB26">
         <v>0.34132089999999998</v>
       </c>
-      <c r="AC25">
+      <c r="AC26">
         <v>0.30310680000000001</v>
       </c>
-      <c r="AD25">
+      <c r="AD26">
         <v>0.38435269999999999</v>
       </c>
-      <c r="AE25" s="3">
+      <c r="AE26" s="3">
         <v>6.029524E-2</v>
       </c>
-      <c r="AF25">
+      <c r="AF26">
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:32" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="24">
-        <v>40</v>
-      </c>
-      <c r="H26" s="24">
-        <v>240</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="K26" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W26" s="27"/>
-      <c r="Y26" s="27"/>
-      <c r="AE26" s="27"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>19</v>
       </c>
@@ -2837,169 +2903,178 @@
       <c r="D27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E27" s="25">
+        <v>2</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="25">
+        <v>40</v>
+      </c>
+      <c r="H27" s="25">
+        <v>240</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="J27" s="25"/>
+      <c r="K27" s="2">
+        <v>43738.974768518521</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>210</v>
+      </c>
+      <c r="N27">
+        <f>O27-O30</f>
+        <v>1641.2622000000001</v>
+      </c>
+      <c r="O27">
+        <v>2182.027</v>
+      </c>
+      <c r="P27">
+        <v>0.23217930000000001</v>
+      </c>
+      <c r="Q27">
+        <v>0.99128780000000005</v>
+      </c>
+      <c r="R27" s="25">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27" s="3">
+        <v>161.60210000000001</v>
+      </c>
+      <c r="U27">
+        <v>149.82069999999999</v>
+      </c>
+      <c r="V27">
+        <v>174.3099</v>
+      </c>
+      <c r="W27" s="3">
+        <v>3.8411479999999998E-2</v>
+      </c>
+      <c r="X27">
+        <v>0.1230586</v>
+      </c>
+      <c r="Y27" s="3">
+        <v>9.4861479999999998E-2</v>
+      </c>
+      <c r="Z27" s="3">
+        <v>0.15963730000000001</v>
+      </c>
+      <c r="AA27">
+        <v>0.13258120000000001</v>
+      </c>
+      <c r="AB27">
+        <v>0.4533896</v>
+      </c>
+      <c r="AC27">
+        <v>0.38975680000000001</v>
+      </c>
+      <c r="AD27">
+        <v>0.52741119999999997</v>
+      </c>
+      <c r="AE27" s="3">
+        <v>7.6822959999999996E-2</v>
+      </c>
+      <c r="AF27">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
         <v>36</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K28" s="2">
         <v>43674.88685185185</v>
       </c>
-      <c r="L27">
-        <v>2</v>
-      </c>
-      <c r="M27">
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
         <v>217</v>
       </c>
-      <c r="N27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O27">
+      <c r="N28">
+        <f>O28-O30</f>
+        <v>1777.3522000000003</v>
+      </c>
+      <c r="O28">
         <v>2318.1170000000002</v>
       </c>
-      <c r="P27">
+      <c r="P28">
         <v>0.14716180000000001</v>
       </c>
-      <c r="Q27">
+      <c r="Q28">
         <v>0.56517220000000001</v>
       </c>
-      <c r="R27">
+      <c r="R28">
         <v>0.7</v>
       </c>
-      <c r="S27">
+      <c r="S28">
         <v>0.6</v>
       </c>
-      <c r="T27">
+      <c r="T28">
         <v>175.25049999999999</v>
       </c>
-      <c r="U27">
+      <c r="U28">
         <v>165.1422</v>
       </c>
-      <c r="V27">
+      <c r="V28">
         <v>185.97749999999999</v>
       </c>
-      <c r="W27" s="3">
+      <c r="W28" s="3">
         <v>3.014762E-2</v>
       </c>
-      <c r="X27">
+      <c r="X28">
         <v>0.1081255</v>
       </c>
-      <c r="Y27" s="3">
+      <c r="Y28" s="3">
         <v>8.4573930000000005E-2</v>
       </c>
-      <c r="Z27">
+      <c r="Z28">
         <v>0.13823550000000001</v>
       </c>
-      <c r="AA27">
+      <c r="AA28">
         <v>0.1249208</v>
       </c>
-      <c r="AB27">
+      <c r="AB28">
         <v>0.34132089999999998</v>
       </c>
-      <c r="AC27">
+      <c r="AC28">
         <v>0.30310680000000001</v>
       </c>
-      <c r="AD27">
+      <c r="AD28">
         <v>0.38435269999999999</v>
       </c>
-      <c r="AE27" s="3">
+      <c r="AE28" s="3">
         <v>6.029524E-2</v>
       </c>
-      <c r="AF27">
+      <c r="AF28">
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:32" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G28" s="24">
-        <v>40</v>
-      </c>
-      <c r="H28" s="24">
-        <v>240</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2">
-        <v>43737.703449074077</v>
-      </c>
-      <c r="L28">
-        <v>2</v>
-      </c>
-      <c r="M28">
-        <v>210</v>
-      </c>
-      <c r="N28">
-        <f>O28-O28</f>
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>540.76480000000004</v>
-      </c>
-      <c r="P28">
-        <v>0.34628930000000002</v>
-      </c>
-      <c r="Q28"/>
-      <c r="R28"/>
-      <c r="S28"/>
-      <c r="T28">
-        <v>160.1337</v>
-      </c>
-      <c r="U28">
-        <v>147.2749</v>
-      </c>
-      <c r="V28">
-        <v>174.11519999999999</v>
-      </c>
-      <c r="W28" s="3">
-        <v>4.2479589999999998E-2</v>
-      </c>
-      <c r="X28">
-        <v>0.12532579999999999</v>
-      </c>
-      <c r="Y28" s="3">
-        <v>9.571064E-2</v>
-      </c>
-      <c r="Z28">
-        <v>0.16410459999999999</v>
-      </c>
-      <c r="AA28">
-        <v>0.13745579999999999</v>
-      </c>
-      <c r="AB28">
-        <v>0.44518770000000002</v>
-      </c>
-      <c r="AC28">
-        <v>0.37664589999999998</v>
-      </c>
-      <c r="AD28">
-        <v>0.52620259999999996</v>
-      </c>
-      <c r="AE28" s="3">
-        <v>8.4959190000000004E-2</v>
-      </c>
-      <c r="AF28">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
@@ -3012,81 +3087,90 @@
       <c r="D29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29" s="2">
-        <v>43674.886793981481</v>
-      </c>
-      <c r="L29">
-        <v>3</v>
-      </c>
-      <c r="M29">
-        <v>217</v>
+      <c r="E29" s="25">
+        <v>2</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="25">
+        <v>40</v>
+      </c>
+      <c r="H29" s="25">
+        <v>240</v>
+      </c>
+      <c r="I29" s="25">
+        <v>4</v>
+      </c>
+      <c r="K29" s="26">
+        <v>43738.960416666669</v>
+      </c>
+      <c r="L29" s="25">
+        <v>2</v>
+      </c>
+      <c r="M29" s="25">
+        <v>210</v>
       </c>
       <c r="N29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>2319.6460000000002</v>
-      </c>
-      <c r="P29">
-        <v>0.10358630000000001</v>
-      </c>
-      <c r="Q29">
-        <v>0.14296420000000001</v>
-      </c>
-      <c r="R29">
-        <v>0.3</v>
-      </c>
-      <c r="S29">
-        <v>0.2</v>
-      </c>
-      <c r="T29">
-        <v>162.1482</v>
-      </c>
-      <c r="U29">
-        <v>133.05889999999999</v>
-      </c>
-      <c r="V29">
-        <v>197.59710000000001</v>
-      </c>
-      <c r="W29">
-        <v>0.10056130000000001</v>
-      </c>
-      <c r="X29">
-        <v>0.12630540000000001</v>
-      </c>
-      <c r="Y29" s="3">
-        <v>8.0956379999999994E-2</v>
-      </c>
-      <c r="Z29">
-        <v>0.1970576</v>
-      </c>
-      <c r="AA29">
-        <v>0.22895399999999999</v>
-      </c>
-      <c r="AB29">
-        <v>0.29219230000000002</v>
-      </c>
-      <c r="AC29">
-        <v>0.1973346</v>
-      </c>
-      <c r="AD29">
-        <v>0.43264770000000002</v>
-      </c>
-      <c r="AE29">
-        <v>0.20112250000000001</v>
-      </c>
-      <c r="AF29">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+        <f>O29-O30</f>
+        <v>1641.2622000000001</v>
+      </c>
+      <c r="O29" s="25">
+        <v>2182.027</v>
+      </c>
+      <c r="P29" s="25">
+        <v>0.23217930000000001</v>
+      </c>
+      <c r="Q29" s="25">
+        <v>0.99128780000000005</v>
+      </c>
+      <c r="R29" s="25">
+        <v>1</v>
+      </c>
+      <c r="S29" s="25">
+        <v>1</v>
+      </c>
+      <c r="T29" s="25">
+        <v>161.60210000000001</v>
+      </c>
+      <c r="U29" s="25">
+        <v>149.82069999999999</v>
+      </c>
+      <c r="V29" s="25">
+        <v>174.3099</v>
+      </c>
+      <c r="W29" s="27">
+        <v>3.8411479999999998E-2</v>
+      </c>
+      <c r="X29" s="25">
+        <v>0.1230586</v>
+      </c>
+      <c r="Y29" s="27">
+        <v>9.4861479999999998E-2</v>
+      </c>
+      <c r="Z29" s="25">
+        <v>0.15963730000000001</v>
+      </c>
+      <c r="AA29" s="25">
+        <v>0.13258120000000001</v>
+      </c>
+      <c r="AB29" s="25">
+        <v>0.4533896</v>
+      </c>
+      <c r="AC29" s="25">
+        <v>0.38975680000000001</v>
+      </c>
+      <c r="AD29" s="25">
+        <v>0.52741119999999997</v>
+      </c>
+      <c r="AE29" s="27">
+        <v>7.6822959999999996E-2</v>
+      </c>
+      <c r="AF29" s="25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
@@ -3099,78 +3183,78 @@
       <c r="D30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30" t="s">
-        <v>37</v>
-      </c>
-      <c r="K30" s="2">
-        <v>43674.886747685188</v>
-      </c>
-      <c r="L30">
-        <v>2</v>
-      </c>
-      <c r="M30">
-        <v>217</v>
+      <c r="E30" s="25">
+        <v>2</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="25">
+        <v>40</v>
+      </c>
+      <c r="H30" s="25">
+        <v>240</v>
+      </c>
+      <c r="J30" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="K30" s="26">
+        <v>43738.960509259261</v>
+      </c>
+      <c r="L30" s="25">
+        <v>2</v>
+      </c>
+      <c r="M30" s="25">
+        <v>210</v>
       </c>
       <c r="N30">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N30" si="1">O30-O30</f>
         <v>0</v>
       </c>
-      <c r="O30">
-        <v>2318.1239999999998</v>
-      </c>
-      <c r="P30" s="3">
-        <v>2.5541129999999999E-2</v>
-      </c>
-      <c r="Q30">
-        <v>0.18720819999999999</v>
-      </c>
-      <c r="R30">
-        <v>0.2</v>
-      </c>
-      <c r="S30">
-        <v>0.15</v>
-      </c>
-      <c r="T30">
-        <v>159.59049999999999</v>
-      </c>
-      <c r="U30">
-        <v>153.6918</v>
-      </c>
-      <c r="V30">
-        <v>165.71559999999999</v>
-      </c>
-      <c r="W30" s="3">
-        <v>1.9109250000000001E-2</v>
-      </c>
-      <c r="X30">
-        <v>0.13038649999999999</v>
-      </c>
-      <c r="Y30">
-        <v>0.10374890000000001</v>
-      </c>
-      <c r="Z30">
-        <v>0.16386329999999999</v>
-      </c>
-      <c r="AA30">
-        <v>0.1158893</v>
-      </c>
-      <c r="AB30">
-        <v>0.28304689999999999</v>
-      </c>
-      <c r="AC30">
-        <v>0.2625152</v>
-      </c>
-      <c r="AD30">
-        <v>0.30518430000000002</v>
-      </c>
-      <c r="AE30" s="3">
-        <v>3.8218509999999997E-2</v>
-      </c>
-      <c r="AF30">
-        <v>215</v>
+      <c r="O30" s="25">
+        <v>540.76480000000004</v>
+      </c>
+      <c r="P30" s="25">
+        <v>0.34628930000000002</v>
+      </c>
+      <c r="T30" s="25">
+        <v>160.1337</v>
+      </c>
+      <c r="U30" s="25">
+        <v>147.2749</v>
+      </c>
+      <c r="V30" s="25">
+        <v>174.11519999999999</v>
+      </c>
+      <c r="W30" s="27">
+        <v>4.2479589999999998E-2</v>
+      </c>
+      <c r="X30" s="25">
+        <v>0.12532579999999999</v>
+      </c>
+      <c r="Y30" s="27">
+        <v>9.571064E-2</v>
+      </c>
+      <c r="Z30" s="25">
+        <v>0.16410459999999999</v>
+      </c>
+      <c r="AA30" s="25">
+        <v>0.13745579999999999</v>
+      </c>
+      <c r="AB30" s="25">
+        <v>0.44518770000000002</v>
+      </c>
+      <c r="AC30" s="25">
+        <v>0.37664589999999998</v>
+      </c>
+      <c r="AD30" s="25">
+        <v>0.52620259999999996</v>
+      </c>
+      <c r="AE30" s="27">
+        <v>8.4959190000000004E-2</v>
+      </c>
+      <c r="AF30" s="25">
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.3">
@@ -3190,10 +3274,10 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K31" s="2">
-        <v>43674.886701388888</v>
+        <v>43674.886793981481</v>
       </c>
       <c r="L31">
         <v>3</v>
@@ -3202,61 +3286,235 @@
         <v>217</v>
       </c>
       <c r="N31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>O31-O30</f>
+        <v>1778.8812000000003</v>
       </c>
       <c r="O31">
+        <v>2319.6460000000002</v>
+      </c>
+      <c r="P31">
+        <v>0.10358630000000001</v>
+      </c>
+      <c r="Q31">
+        <v>0.14296420000000001</v>
+      </c>
+      <c r="R31">
+        <v>0.3</v>
+      </c>
+      <c r="S31">
+        <v>0.2</v>
+      </c>
+      <c r="T31">
+        <v>162.1482</v>
+      </c>
+      <c r="U31">
+        <v>133.05889999999999</v>
+      </c>
+      <c r="V31">
+        <v>197.59710000000001</v>
+      </c>
+      <c r="W31">
+        <v>0.10056130000000001</v>
+      </c>
+      <c r="X31">
+        <v>0.12630540000000001</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>8.0956379999999994E-2</v>
+      </c>
+      <c r="Z31">
+        <v>0.1970576</v>
+      </c>
+      <c r="AA31">
+        <v>0.22895399999999999</v>
+      </c>
+      <c r="AB31">
+        <v>0.29219230000000002</v>
+      </c>
+      <c r="AC31">
+        <v>0.1973346</v>
+      </c>
+      <c r="AD31">
+        <v>0.43264770000000002</v>
+      </c>
+      <c r="AE31">
+        <v>0.20112250000000001</v>
+      </c>
+      <c r="AF31">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="2">
+        <v>43674.886747685188</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="M32">
+        <v>217</v>
+      </c>
+      <c r="N32">
+        <f>O32-O30</f>
+        <v>1777.3591999999999</v>
+      </c>
+      <c r="O32">
+        <v>2318.1239999999998</v>
+      </c>
+      <c r="P32" s="3">
+        <v>2.5541129999999999E-2</v>
+      </c>
+      <c r="Q32">
+        <v>0.18720819999999999</v>
+      </c>
+      <c r="R32">
+        <v>0.2</v>
+      </c>
+      <c r="S32">
+        <v>0.15</v>
+      </c>
+      <c r="T32">
+        <v>159.59049999999999</v>
+      </c>
+      <c r="U32">
+        <v>153.6918</v>
+      </c>
+      <c r="V32">
+        <v>165.71559999999999</v>
+      </c>
+      <c r="W32" s="3">
+        <v>1.9109250000000001E-2</v>
+      </c>
+      <c r="X32">
+        <v>0.13038649999999999</v>
+      </c>
+      <c r="Y32">
+        <v>0.10374890000000001</v>
+      </c>
+      <c r="Z32">
+        <v>0.16386329999999999</v>
+      </c>
+      <c r="AA32">
+        <v>0.1158893</v>
+      </c>
+      <c r="AB32">
+        <v>0.28304689999999999</v>
+      </c>
+      <c r="AC32">
+        <v>0.2625152</v>
+      </c>
+      <c r="AD32">
+        <v>0.30518430000000002</v>
+      </c>
+      <c r="AE32" s="3">
+        <v>3.8218509999999997E-2</v>
+      </c>
+      <c r="AF32">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="2">
+        <v>43674.886701388888</v>
+      </c>
+      <c r="L33">
+        <v>3</v>
+      </c>
+      <c r="M33">
+        <v>217</v>
+      </c>
+      <c r="N33">
+        <f>O33-O30</f>
+        <v>1777.9572000000003</v>
+      </c>
+      <c r="O33">
         <v>2318.7220000000002</v>
       </c>
-      <c r="P31">
+      <c r="P33">
         <v>0.1377823</v>
       </c>
-      <c r="Q31">
+      <c r="Q33">
         <v>0.37579010000000002</v>
       </c>
-      <c r="R31">
+      <c r="R33">
         <v>0.6</v>
       </c>
-      <c r="S31">
+      <c r="S33">
         <v>0.4</v>
       </c>
-      <c r="T31">
+      <c r="T33">
         <v>170.42619999999999</v>
       </c>
-      <c r="U31">
+      <c r="U33">
         <v>114.8938</v>
       </c>
-      <c r="V31">
+      <c r="V33">
         <v>252.79939999999999</v>
       </c>
-      <c r="W31">
+      <c r="W33">
         <v>0.20205419999999999</v>
       </c>
-      <c r="X31">
+      <c r="X33">
         <v>0.11433359999999999</v>
       </c>
-      <c r="Y31" s="3">
+      <c r="Y33" s="3">
         <v>5.1807619999999999E-2</v>
       </c>
-      <c r="Z31">
+      <c r="Z33">
         <v>0.25232149999999998</v>
       </c>
-      <c r="AA31">
+      <c r="AA33">
         <v>0.41865659999999999</v>
       </c>
-      <c r="AB31">
+      <c r="AB33">
         <v>0.32278760000000001</v>
       </c>
-      <c r="AC31">
+      <c r="AC33">
         <v>0.14996119999999999</v>
       </c>
-      <c r="AD31">
+      <c r="AD33">
         <v>0.69479199999999997</v>
       </c>
-      <c r="AE31">
+      <c r="AE33">
         <v>0.40410849999999998</v>
       </c>
-      <c r="AF31">
+      <c r="AF33">
         <v>214</v>
       </c>
     </row>
@@ -3288,10 +3546,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE24CEF8-8E3C-4A9E-BBF1-3AAF52D2BA4B}">
-  <dimension ref="A1:BF35"/>
+  <dimension ref="G1:CC35"/>
   <sheetViews>
-    <sheetView topLeftCell="AC13" workbookViewId="0">
-      <selection activeCell="AJ31" sqref="AJ31:BF31"/>
+    <sheetView topLeftCell="BS1" workbookViewId="0">
+      <selection activeCell="BG7" sqref="BG7:CC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3299,1894 +3557,1427 @@
     <col min="6" max="6" width="19.5546875" customWidth="1"/>
     <col min="20" max="20" width="19.5546875" customWidth="1"/>
     <col min="34" max="34" width="24.77734375" customWidth="1"/>
+    <col min="35" max="35" width="9" customWidth="1"/>
+    <col min="36" max="36" width="17.109375" customWidth="1"/>
+    <col min="39" max="39" width="23.6640625" customWidth="1"/>
+    <col min="41" max="41" width="17.21875" customWidth="1"/>
+    <col min="57" max="57" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="AC1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="AC2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="AH2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="AC4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="AE4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="AI4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" t="s">
+      <c r="AK4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s">
+      <c r="AL4" t="s">
         <v>74</v>
       </c>
-      <c r="E4" t="s">
+      <c r="AM4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN4" t="s">
         <v>75</v>
       </c>
-      <c r="F4" t="s">
+      <c r="AO4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>72</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>74</v>
+      </c>
+      <c r="BE4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
+      <c r="BF4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH4" t="s">
         <v>76</v>
       </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="BI4" t="s">
         <v>23</v>
       </c>
-      <c r="K4" t="s">
+      <c r="BJ4" t="s">
         <v>44</v>
       </c>
-      <c r="L4" t="s">
+      <c r="BK4" t="s">
         <v>24</v>
       </c>
-      <c r="M4" t="s">
+      <c r="BL4" t="s">
         <v>25</v>
       </c>
-      <c r="N4" t="s">
+      <c r="BM4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" t="s">
+      <c r="BN4" t="s">
         <v>50</v>
       </c>
-      <c r="P4" t="s">
+      <c r="BO4" t="s">
         <v>49</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="BP4" t="s">
         <v>48</v>
       </c>
-      <c r="R4" t="s">
+      <c r="BQ4" t="s">
         <v>28</v>
       </c>
-      <c r="S4" t="s">
+      <c r="BR4" t="s">
         <v>29</v>
       </c>
-      <c r="T4" t="s">
+      <c r="BS4" t="s">
         <v>30</v>
       </c>
-      <c r="U4" t="s">
+      <c r="BT4" t="s">
         <v>55</v>
       </c>
-      <c r="V4" t="s">
+      <c r="BU4" t="s">
         <v>31</v>
       </c>
-      <c r="W4" t="s">
+      <c r="BV4" t="s">
         <v>32</v>
       </c>
-      <c r="X4" t="s">
+      <c r="BW4" t="s">
         <v>33</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="BX4" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="BY4" t="s">
         <v>51</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="BZ4" t="s">
         <v>52</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="CA4" t="s">
         <v>53</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="CB4" t="s">
         <v>56</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="CC4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="U5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="AC5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>5</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>5</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>5</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>5</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>43645.731585648151</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>43674.886631944442</v>
+      </c>
+      <c r="AP5">
+        <v>5</v>
+      </c>
+      <c r="AQ5">
+        <v>2</v>
+      </c>
+      <c r="AR5">
+        <v>217</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>2318.1170000000002</v>
+      </c>
+      <c r="AU5">
+        <v>0.14716180000000001</v>
+      </c>
+      <c r="AV5">
+        <v>0.56517220000000001</v>
+      </c>
+      <c r="AW5" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AX5">
+        <v>0.6</v>
+      </c>
+      <c r="AY5" s="3">
+        <v>175.25049999999999</v>
+      </c>
+      <c r="AZ5">
+        <v>1</v>
+      </c>
+      <c r="BA5">
         <v>6</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
+      <c r="BB5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC5">
+        <v>2</v>
+      </c>
+      <c r="BD5" s="3">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="BE5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF5" s="2">
         <v>43737.672731481478</v>
       </c>
-      <c r="H5" s="2">
+      <c r="BG5" s="2">
         <v>43737.674988425926</v>
       </c>
-      <c r="I5">
+      <c r="BH5">
         <v>6</v>
       </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
+      <c r="BI5">
+        <v>2</v>
+      </c>
+      <c r="BJ5" s="3">
         <v>215</v>
       </c>
-      <c r="L5">
+      <c r="BK5">
         <v>0</v>
       </c>
-      <c r="M5">
+      <c r="BL5">
         <v>2270.0810000000001</v>
       </c>
-      <c r="N5">
+      <c r="BM5">
         <v>0.69110099999999997</v>
       </c>
-      <c r="O5">
+      <c r="BN5">
         <v>0.92968229999999996</v>
       </c>
-      <c r="P5">
+      <c r="BO5">
         <v>0.9</v>
       </c>
-      <c r="Q5">
+      <c r="BP5">
         <v>0.9</v>
       </c>
-      <c r="R5">
+      <c r="BQ5">
         <v>166.21420000000001</v>
       </c>
-      <c r="S5">
+      <c r="BR5">
         <v>155.69970000000001</v>
       </c>
-      <c r="T5">
+      <c r="BS5">
         <v>177.43879999999999</v>
       </c>
-      <c r="U5" s="3">
+      <c r="BT5" s="3">
         <v>3.3161290000000003E-2</v>
       </c>
-      <c r="V5">
+      <c r="BU5">
         <v>0.1190937</v>
       </c>
-      <c r="W5" s="3">
+      <c r="BV5" s="3">
         <v>9.2797210000000005E-2</v>
       </c>
-      <c r="X5">
+      <c r="BW5">
         <v>0.15284200000000001</v>
       </c>
-      <c r="Y5">
+      <c r="BX5">
         <v>0.12695770000000001</v>
       </c>
-      <c r="Z5">
+      <c r="BY5">
         <v>0.30696859999999998</v>
       </c>
-      <c r="AA5">
+      <c r="BZ5">
         <v>0.26938889999999999</v>
       </c>
-      <c r="AB5">
+      <c r="CA5">
         <v>0.34979060000000001</v>
       </c>
-      <c r="AC5" s="3">
+      <c r="CB5" s="3">
         <v>6.6322569999999997E-2</v>
       </c>
-      <c r="AD5">
+      <c r="CC5">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="U6" s="3"/>
+      <c r="AC6" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD6">
+        <v>7</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>3</v>
+      </c>
+      <c r="AG6">
+        <v>7</v>
+      </c>
+      <c r="AH6">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>8</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <v>3</v>
+      </c>
+      <c r="AL6">
+        <v>8</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>43738.970381944448</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>43738.974768518521</v>
+      </c>
+      <c r="AP6">
+        <v>8</v>
+      </c>
+      <c r="AQ6">
+        <v>2</v>
+      </c>
+      <c r="AR6">
+        <v>210</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>2182.027</v>
+      </c>
+      <c r="AU6">
+        <v>0.23217930000000001</v>
+      </c>
+      <c r="AV6">
+        <v>0.99128780000000005</v>
+      </c>
+      <c r="AW6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AX6">
+        <v>1</v>
+      </c>
+      <c r="AY6" s="3">
+        <v>161.60210000000001</v>
+      </c>
+      <c r="AZ6">
+        <v>1</v>
+      </c>
+      <c r="BA6">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
+      <c r="BB6" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC6">
+        <v>1</v>
+      </c>
+      <c r="BD6" s="3">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
+      <c r="BE6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="2">
+      <c r="BF6" s="2">
         <v>43645.731585648151</v>
       </c>
-      <c r="H6" s="2">
+      <c r="BG6" s="2">
         <v>43674.877928240741</v>
       </c>
-      <c r="I6">
+      <c r="BH6">
         <v>5</v>
       </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6">
+      <c r="BI6">
+        <v>2</v>
+      </c>
+      <c r="BJ6" s="3">
         <v>217</v>
       </c>
-      <c r="L6">
+      <c r="BK6">
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="BL6">
         <v>2318.1190000000001</v>
       </c>
-      <c r="N6">
+      <c r="BM6">
         <v>0.14708280000000001</v>
       </c>
-      <c r="O6">
+      <c r="BN6">
         <v>0.56151450000000003</v>
       </c>
-      <c r="P6">
+      <c r="BO6">
         <v>0.7</v>
       </c>
-      <c r="Q6">
+      <c r="BP6">
         <v>0.6</v>
       </c>
-      <c r="R6">
+      <c r="BQ6">
         <v>175.24680000000001</v>
       </c>
-      <c r="S6">
+      <c r="BR6">
         <v>165.1386</v>
       </c>
-      <c r="T6">
+      <c r="BS6">
         <v>185.97370000000001</v>
       </c>
-      <c r="U6" s="3">
+      <c r="BT6" s="3">
         <v>3.0148089999999999E-2</v>
       </c>
-      <c r="V6">
+      <c r="BU6">
         <v>0.10813</v>
       </c>
-      <c r="W6">
+      <c r="BV6">
         <v>8.4577399999999997E-2</v>
       </c>
-      <c r="X6">
+      <c r="BW6">
         <v>0.13824139999999999</v>
       </c>
-      <c r="Y6">
+      <c r="BX6">
         <v>0.1249212</v>
       </c>
-      <c r="Z6">
+      <c r="BY6">
         <v>0.34123829999999999</v>
       </c>
-      <c r="AA6">
+      <c r="BZ6">
         <v>0.30303289999999999</v>
       </c>
-      <c r="AB6">
+      <c r="CA6">
         <v>0.3842604</v>
       </c>
-      <c r="AC6" s="3">
+      <c r="CB6" s="3">
         <v>6.0296170000000003E-2</v>
       </c>
-      <c r="AD6">
+      <c r="CC6">
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="U7" s="3"/>
+      <c r="AC7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD7">
+        <v>6</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>2</v>
+      </c>
+      <c r="AG7">
+        <v>6</v>
+      </c>
+      <c r="AH7">
+        <v>2</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>7</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK7">
+        <v>3</v>
+      </c>
+      <c r="AL7">
+        <v>7</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>43738.93545138889</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>43738.960416666669</v>
+      </c>
+      <c r="AP7">
+        <v>7</v>
+      </c>
+      <c r="AQ7">
+        <v>2</v>
+      </c>
+      <c r="AR7">
+        <v>210</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>2182.027</v>
+      </c>
+      <c r="AU7">
+        <v>0.23217930000000001</v>
+      </c>
+      <c r="AV7">
+        <v>0.99128780000000005</v>
+      </c>
+      <c r="AW7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AX7">
+        <v>1</v>
+      </c>
+      <c r="AY7" s="3">
+        <v>161.60210000000001</v>
+      </c>
+      <c r="AZ7">
+        <v>2</v>
+      </c>
+      <c r="BA7">
+        <v>7</v>
+      </c>
+      <c r="BB7" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC7">
+        <v>3</v>
+      </c>
+      <c r="BD7" s="3">
+        <v>6</v>
+      </c>
+      <c r="BE7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BF7" s="2">
+        <v>43739.626145833332</v>
+      </c>
+      <c r="BG7" s="2">
+        <v>43739.628611111111</v>
+      </c>
+      <c r="BH7">
+        <v>7</v>
+      </c>
+      <c r="BI7">
+        <v>2</v>
+      </c>
+      <c r="BJ7" s="3">
+        <v>210</v>
+      </c>
+      <c r="BK7">
+        <v>0</v>
+      </c>
+      <c r="BL7">
+        <v>540.76530000000002</v>
+      </c>
+      <c r="BM7">
+        <v>0.34615800000000002</v>
+      </c>
+      <c r="BQ7">
+        <v>160.13</v>
+      </c>
+      <c r="BR7">
+        <v>147.26949999999999</v>
+      </c>
+      <c r="BS7">
+        <v>174.11349999999999</v>
+      </c>
+      <c r="BT7" s="3">
+        <v>4.2486370000000002E-2</v>
+      </c>
+      <c r="BU7">
+        <v>0.12533159999999999</v>
+      </c>
+      <c r="BV7" s="3">
+        <v>9.5713560000000003E-2</v>
+      </c>
+      <c r="BW7">
+        <v>0.16411490000000001</v>
+      </c>
+      <c r="BX7">
+        <v>0.13746410000000001</v>
+      </c>
+      <c r="BY7">
+        <v>0.44516689999999998</v>
+      </c>
+      <c r="BZ7">
+        <v>0.37661830000000002</v>
+      </c>
+      <c r="CA7">
+        <v>0.52619210000000005</v>
+      </c>
+      <c r="CB7" s="3">
+        <v>8.497275E-2</v>
+      </c>
+      <c r="CC7">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="AC8" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD8">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="AH8">
+        <v>2</v>
+      </c>
+      <c r="AI8" s="2">
+        <v>6</v>
+      </c>
+      <c r="AJ8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>2</v>
+      </c>
+      <c r="AL8">
+        <v>6</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>43737.68613425926</v>
+      </c>
+      <c r="AO8" s="2">
+        <v>43738.960509259261</v>
+      </c>
+      <c r="AP8">
+        <v>6</v>
+      </c>
+      <c r="AQ8">
+        <v>2</v>
+      </c>
+      <c r="AR8">
+        <v>210</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>540.76480000000004</v>
+      </c>
+      <c r="AU8">
+        <v>0.34628930000000002</v>
+      </c>
+      <c r="AW8" s="3"/>
+      <c r="AY8" s="3">
+        <v>160.1337</v>
+      </c>
+      <c r="AZ8">
+        <v>2</v>
+      </c>
+      <c r="BA8">
+        <v>4</v>
+      </c>
+      <c r="BB8" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC8">
+        <v>1</v>
+      </c>
+      <c r="BD8" s="3">
+        <v>4</v>
+      </c>
+      <c r="BE8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="2">
+      <c r="BF8" s="2">
         <v>43645.728414351855</v>
       </c>
-      <c r="H7" s="2">
+      <c r="BG8" s="2">
         <v>43674.878622685188</v>
       </c>
-      <c r="I7">
+      <c r="BH8">
         <v>4</v>
       </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7">
+      <c r="BI8">
+        <v>2</v>
+      </c>
+      <c r="BJ8" s="3">
         <v>217</v>
       </c>
-      <c r="L7">
+      <c r="BK8">
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="BL8">
         <v>2318.1190000000001</v>
       </c>
-      <c r="N7">
+      <c r="BM8">
         <v>0.14708280000000001</v>
       </c>
-      <c r="O7">
+      <c r="BN8">
         <v>0.56151450000000003</v>
       </c>
-      <c r="P7">
+      <c r="BO8">
         <v>0.7</v>
       </c>
-      <c r="Q7">
+      <c r="BP8">
         <v>0.6</v>
       </c>
-      <c r="R7">
+      <c r="BQ8">
         <v>175.24680000000001</v>
       </c>
-      <c r="S7">
+      <c r="BR8">
         <v>165.1386</v>
       </c>
-      <c r="T7">
+      <c r="BS8">
         <v>185.97370000000001</v>
       </c>
-      <c r="U7" s="3">
+      <c r="BT8" s="3">
         <v>3.0148089999999999E-2</v>
       </c>
-      <c r="V7">
+      <c r="BU8">
         <v>0.10813</v>
       </c>
-      <c r="W7">
+      <c r="BV8">
         <v>8.4577399999999997E-2</v>
       </c>
-      <c r="X7">
+      <c r="BW8">
         <v>0.13824139999999999</v>
       </c>
-      <c r="Y7">
+      <c r="BX8">
         <v>0.1249212</v>
       </c>
-      <c r="Z7">
+      <c r="BY8">
         <v>0.34123829999999999</v>
       </c>
-      <c r="AA7">
+      <c r="BZ8">
         <v>0.30303289999999999</v>
       </c>
-      <c r="AB7">
+      <c r="CA8">
         <v>0.3842604</v>
       </c>
-      <c r="AC7" s="3">
+      <c r="CB8" s="3">
         <v>6.0296170000000003E-2</v>
       </c>
-      <c r="AD7">
+      <c r="CC8">
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
+    <row r="9" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="L9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="AC9" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD9">
         <v>3</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
+      <c r="AH9">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="2">
+        <v>4</v>
+      </c>
+      <c r="AJ9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>4</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>43645.728414351855</v>
+      </c>
+      <c r="AO9" s="2">
+        <v>43674.88685185185</v>
+      </c>
+      <c r="AP9">
+        <v>4</v>
+      </c>
+      <c r="AQ9">
+        <v>2</v>
+      </c>
+      <c r="AR9">
+        <v>217</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>2318.1170000000002</v>
+      </c>
+      <c r="AU9">
+        <v>0.14716180000000001</v>
+      </c>
+      <c r="AV9">
+        <v>0.56517220000000001</v>
+      </c>
+      <c r="AW9">
+        <v>0.7</v>
+      </c>
+      <c r="AX9">
+        <v>0.6</v>
+      </c>
+      <c r="AY9" s="3">
+        <v>175.25049999999999</v>
+      </c>
+      <c r="AZ9">
+        <v>2</v>
+      </c>
+      <c r="BA9">
+        <v>3</v>
+      </c>
+      <c r="BB9" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC9">
+        <v>1</v>
+      </c>
+      <c r="BD9" s="3">
+        <v>3</v>
+      </c>
+      <c r="BE9" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="2">
+      <c r="BF9" s="2">
         <v>43645.720439814817</v>
       </c>
-      <c r="H8" s="2">
+      <c r="BG9" s="2">
         <v>43674.878668981481</v>
       </c>
-      <c r="I8">
+      <c r="BH9">
         <v>3</v>
       </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8">
+      <c r="BI9">
+        <v>2</v>
+      </c>
+      <c r="BJ9" s="3">
         <v>217</v>
       </c>
-      <c r="L8">
+      <c r="BK9">
         <v>9.4890139999999992</v>
       </c>
-      <c r="M8">
+      <c r="BL9">
         <v>2327.6080000000002</v>
       </c>
-      <c r="N8" s="3">
+      <c r="BM9" s="3">
         <v>3.3778610000000001E-2</v>
       </c>
-      <c r="O8" s="3">
+      <c r="BN9" s="3">
         <v>2.1573459999999999E-2</v>
       </c>
-      <c r="P8">
+      <c r="BO9">
         <v>0.1</v>
       </c>
-      <c r="Q8">
+      <c r="BP9">
         <v>0.05</v>
       </c>
-      <c r="R8">
+      <c r="BQ9">
         <v>146.255</v>
       </c>
-      <c r="S8">
+      <c r="BR9">
         <v>133.4556</v>
       </c>
-      <c r="T8">
+      <c r="BS9">
         <v>160.28190000000001</v>
       </c>
-      <c r="U8" s="3">
+      <c r="BT9" s="3">
         <v>4.6488710000000003E-2</v>
       </c>
-      <c r="V8">
+      <c r="BU9">
         <v>0.15524769999999999</v>
       </c>
-      <c r="W8">
+      <c r="BV9">
         <v>0.1171735</v>
       </c>
-      <c r="X8">
+      <c r="BW9">
         <v>0.2056935</v>
       </c>
-      <c r="Y8">
+      <c r="BX9">
         <v>0.1435775</v>
       </c>
-      <c r="Z8">
+      <c r="BY9">
         <v>0.23767250000000001</v>
       </c>
-      <c r="AA8">
+      <c r="BZ9">
         <v>0.19795189999999999</v>
       </c>
-      <c r="AB8">
+      <c r="CA9">
         <v>0.28536339999999999</v>
       </c>
-      <c r="AC8" s="3">
+      <c r="CB9" s="3">
         <v>9.297743E-2</v>
       </c>
-      <c r="AD8">
+      <c r="CC9">
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
+    <row r="10" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="W10" s="3"/>
+      <c r="AC10">
+        <v>2</v>
+      </c>
+      <c r="AD10">
+        <v>2</v>
+      </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>2</v>
+      </c>
+      <c r="AH10">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>3</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN10" s="2">
+        <v>43645.720439814817</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>43674.886793981481</v>
+      </c>
+      <c r="AP10" s="3">
+        <v>3</v>
+      </c>
+      <c r="AQ10">
+        <v>3</v>
+      </c>
+      <c r="AR10">
+        <v>217</v>
+      </c>
+      <c r="AS10">
+        <v>1.529053</v>
+      </c>
+      <c r="AT10">
+        <v>2319.6460000000002</v>
+      </c>
+      <c r="AU10">
+        <v>0.10358630000000001</v>
+      </c>
+      <c r="AV10">
+        <v>0.14296420000000001</v>
+      </c>
+      <c r="AW10" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AX10">
+        <v>0.2</v>
+      </c>
+      <c r="AY10">
+        <v>162.1482</v>
+      </c>
+      <c r="AZ10">
+        <v>2</v>
+      </c>
+      <c r="BA10">
+        <v>2</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
+      <c r="BC10">
+        <v>1</v>
+      </c>
+      <c r="BD10" s="3">
+        <v>2</v>
+      </c>
+      <c r="BE10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="2">
+      <c r="BF10" s="2">
         <v>43645.717662037037</v>
       </c>
-      <c r="H9" s="2">
+      <c r="BG10" s="2">
         <v>43674.878692129627</v>
       </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9">
+      <c r="BH10">
+        <v>2</v>
+      </c>
+      <c r="BI10">
+        <v>2</v>
+      </c>
+      <c r="BJ10">
         <v>217</v>
       </c>
-      <c r="L9" s="3">
+      <c r="BK10" s="3">
         <v>2.0019530000000001E-2</v>
       </c>
-      <c r="M9">
+      <c r="BL10">
         <v>2318.1390000000001</v>
       </c>
-      <c r="N9" s="3">
+      <c r="BM10" s="3">
         <v>2.5966110000000001E-2</v>
       </c>
-      <c r="O9">
+      <c r="BN10">
         <v>0.19065989999999999</v>
       </c>
-      <c r="P9">
+      <c r="BO10">
         <v>0.2</v>
       </c>
-      <c r="Q9">
+      <c r="BP10">
         <v>0.15</v>
       </c>
-      <c r="R9">
+      <c r="BQ10">
         <v>159.67529999999999</v>
       </c>
-      <c r="S9">
+      <c r="BR10">
         <v>153.85550000000001</v>
       </c>
-      <c r="T9">
+      <c r="BS10">
         <v>165.71530000000001</v>
       </c>
-      <c r="U9" s="3">
+      <c r="BT10" s="3">
         <v>1.883862E-2</v>
       </c>
-      <c r="V9">
+      <c r="BU10">
         <v>0.130248</v>
       </c>
-      <c r="W9">
+      <c r="BV10">
         <v>0.1036734</v>
       </c>
-      <c r="X9">
+      <c r="BW10">
         <v>0.16363449999999999</v>
       </c>
-      <c r="Y9">
+      <c r="BX10">
         <v>0.115712</v>
       </c>
-      <c r="Z9">
+      <c r="BY10">
         <v>0.28329110000000002</v>
       </c>
-      <c r="AA9">
+      <c r="BZ10">
         <v>0.26302189999999998</v>
       </c>
-      <c r="AB9">
+      <c r="CA10">
         <v>0.30512230000000001</v>
       </c>
-      <c r="AC9" s="3">
+      <c r="CB10" s="3">
         <v>3.7677240000000001E-2</v>
       </c>
-      <c r="AD9">
+      <c r="CC10">
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
+    <row r="11" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="AC11">
+        <v>2</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AE11">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK11">
+        <v>1</v>
+      </c>
+      <c r="AL11">
+        <v>2</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>43645.717662037037</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>43674.886747685188</v>
+      </c>
+      <c r="AP11">
+        <v>2</v>
+      </c>
+      <c r="AQ11">
+        <v>2</v>
+      </c>
+      <c r="AR11">
+        <v>217</v>
+      </c>
+      <c r="AS11" s="3">
+        <v>7.0800780000000001E-3</v>
+      </c>
+      <c r="AT11">
+        <v>2318.1239999999998</v>
+      </c>
+      <c r="AU11" s="3">
+        <v>2.5541129999999999E-2</v>
+      </c>
+      <c r="AV11">
+        <v>0.18720819999999999</v>
+      </c>
+      <c r="AW11">
+        <v>0.2</v>
+      </c>
+      <c r="AX11">
+        <v>0.15</v>
+      </c>
+      <c r="AY11" s="3">
+        <v>159.59049999999999</v>
+      </c>
+      <c r="AZ11">
+        <v>2</v>
+      </c>
+      <c r="BA11">
+        <v>1</v>
+      </c>
+      <c r="BB11" s="3">
+        <v>1</v>
+      </c>
+      <c r="BC11">
+        <v>1</v>
+      </c>
+      <c r="BD11">
+        <v>1</v>
+      </c>
+      <c r="BE11" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="2">
+      <c r="BF11" s="2">
         <v>43645.697106481479</v>
       </c>
-      <c r="H10" s="2">
+      <c r="BG11" s="2">
         <v>43674.878877314812</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
+      <c r="BH11">
+        <v>1</v>
+      </c>
+      <c r="BI11">
         <v>3</v>
       </c>
-      <c r="K10">
+      <c r="BJ11" s="3">
         <v>217</v>
       </c>
-      <c r="L10">
+      <c r="BK11">
         <v>0.60717770000000004</v>
       </c>
-      <c r="M10">
+      <c r="BL11">
         <v>2318.7260000000001</v>
       </c>
-      <c r="N10">
+      <c r="BM11">
         <v>0.1377766</v>
       </c>
-      <c r="O10">
+      <c r="BN11">
         <v>0.37742910000000002</v>
       </c>
-      <c r="P10">
+      <c r="BO11">
         <v>0.6</v>
       </c>
-      <c r="Q10">
+      <c r="BP11">
         <v>0.4</v>
       </c>
-      <c r="R10">
+      <c r="BQ11">
         <v>170.41839999999999</v>
       </c>
-      <c r="S10">
+      <c r="BR11">
         <v>114.8882</v>
       </c>
-      <c r="T10">
+      <c r="BS11">
         <v>252.7886</v>
       </c>
-      <c r="U10">
+      <c r="BT11">
         <v>0.20205590000000001</v>
       </c>
-      <c r="V10">
+      <c r="BU11">
         <v>0.1143441</v>
       </c>
-      <c r="W10" s="3">
+      <c r="BV11" s="3">
         <v>5.1812080000000003E-2</v>
       </c>
-      <c r="X10">
+      <c r="BW11">
         <v>0.25234600000000001</v>
       </c>
-      <c r="Y10">
+      <c r="BX11">
         <v>0.41865970000000002</v>
       </c>
-      <c r="Z10">
+      <c r="BY11">
         <v>0.32269350000000002</v>
       </c>
-      <c r="AA10">
+      <c r="BZ11">
         <v>0.14991670000000001</v>
       </c>
-      <c r="AB10">
+      <c r="CA11">
         <v>0.69459329999999997</v>
       </c>
-      <c r="AC10">
+      <c r="CB11">
         <v>0.40411170000000002</v>
       </c>
-      <c r="AD10">
+      <c r="CC11">
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="O15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="O16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="O18" t="s">
-        <v>20</v>
-      </c>
-      <c r="P18" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>73</v>
-      </c>
-      <c r="R18" t="s">
-        <v>74</v>
-      </c>
-      <c r="S18" t="s">
-        <v>75</v>
-      </c>
-      <c r="T18" t="s">
-        <v>21</v>
-      </c>
-      <c r="U18" t="s">
-        <v>76</v>
-      </c>
-      <c r="V18" t="s">
-        <v>22</v>
-      </c>
-      <c r="W18" t="s">
-        <v>77</v>
-      </c>
-      <c r="X18" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM18" t="s">
-        <v>27</v>
-      </c>
-      <c r="AN18" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO18" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ18" t="s">
-        <v>56</v>
-      </c>
-      <c r="AR18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="O19">
-        <v>1</v>
-      </c>
-      <c r="P19">
-        <v>6</v>
-      </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-      <c r="R19">
-        <v>2</v>
-      </c>
-      <c r="S19">
-        <v>6</v>
-      </c>
-      <c r="T19" t="s">
-        <v>80</v>
-      </c>
-      <c r="U19" s="2">
-        <v>43737.677662037036</v>
-      </c>
-      <c r="V19" s="2">
-        <v>43737.680763888886</v>
-      </c>
-      <c r="W19">
-        <v>6</v>
-      </c>
-      <c r="X19">
-        <v>1</v>
-      </c>
-      <c r="Y19">
-        <v>387</v>
-      </c>
-      <c r="Z19">
-        <v>0</v>
-      </c>
-      <c r="AA19">
-        <v>4083.6370000000002</v>
-      </c>
-      <c r="AB19">
-        <v>0.43802000000000002</v>
-      </c>
-      <c r="AC19">
-        <v>0.88677879999999998</v>
-      </c>
-      <c r="AD19">
-        <v>0.8</v>
-      </c>
-      <c r="AE19">
-        <v>0.8</v>
-      </c>
-      <c r="AF19">
-        <v>115.56610000000001</v>
-      </c>
-      <c r="AG19">
-        <v>109.70820000000001</v>
-      </c>
-      <c r="AH19">
-        <v>121.73690000000001</v>
-      </c>
-      <c r="AI19" s="3">
-        <v>2.646223E-2</v>
-      </c>
-      <c r="AJ19">
-        <v>0.44344169999999999</v>
-      </c>
-      <c r="AK19">
-        <v>0.37826480000000001</v>
-      </c>
-      <c r="AL19">
-        <v>0.51984909999999995</v>
-      </c>
-      <c r="AM19" s="3">
-        <v>8.0883239999999995E-2</v>
-      </c>
-      <c r="AN19">
-        <v>0.14839479999999999</v>
-      </c>
-      <c r="AO19">
-        <v>0.13373930000000001</v>
-      </c>
-      <c r="AP19">
-        <v>0.1646562</v>
-      </c>
-      <c r="AQ19" s="3">
-        <v>5.292446E-2</v>
-      </c>
-      <c r="AR19">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="20" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20">
-        <v>5</v>
-      </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-      <c r="S20">
-        <v>5</v>
-      </c>
-      <c r="T20" t="s">
-        <v>35</v>
-      </c>
-      <c r="U20" s="2">
-        <v>43645.731585648151</v>
-      </c>
-      <c r="V20" s="2">
-        <v>43648.642766203702</v>
-      </c>
-      <c r="W20">
-        <v>5</v>
-      </c>
-      <c r="X20">
-        <v>2</v>
-      </c>
-      <c r="Y20">
-        <v>423</v>
-      </c>
-      <c r="Z20">
-        <v>10.12842</v>
-      </c>
-      <c r="AA20">
-        <v>4658.0529999999999</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>9.495199E-2</v>
-      </c>
-      <c r="AC20">
-        <v>0.26241229999999999</v>
-      </c>
-      <c r="AD20">
-        <v>0.2</v>
-      </c>
-      <c r="AE20">
-        <v>0.2</v>
-      </c>
-      <c r="AF20">
-        <v>136.4796</v>
-      </c>
-      <c r="AG20">
-        <v>129.1413</v>
-      </c>
-      <c r="AH20">
-        <v>144.23500000000001</v>
-      </c>
-      <c r="AI20" s="3">
-        <v>2.812332E-2</v>
-      </c>
-      <c r="AJ20">
-        <v>0.34752929999999999</v>
-      </c>
-      <c r="AK20">
-        <v>0.29697499999999999</v>
-      </c>
-      <c r="AL20">
-        <v>0.40668959999999998</v>
-      </c>
-      <c r="AM20" s="3">
-        <v>8.0036189999999993E-2</v>
-      </c>
-      <c r="AN20" s="3">
-        <v>7.450677E-2</v>
-      </c>
-      <c r="AO20" s="3">
-        <v>6.6714209999999996E-2</v>
-      </c>
-      <c r="AP20" s="3">
-        <v>8.3209539999999999E-2</v>
-      </c>
-      <c r="AQ20" s="3">
-        <v>5.6246640000000001E-2</v>
-      </c>
-      <c r="AR20">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="21" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>4</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-      <c r="S21">
-        <v>4</v>
-      </c>
-      <c r="T21" t="s">
-        <v>36</v>
-      </c>
-      <c r="U21" s="2">
-        <v>43645.728414351855</v>
-      </c>
-      <c r="V21" s="2">
-        <v>43648.642789351848</v>
-      </c>
-      <c r="W21">
-        <v>4</v>
-      </c>
-      <c r="X21">
-        <v>2</v>
-      </c>
-      <c r="Y21">
-        <v>423</v>
-      </c>
-      <c r="Z21">
-        <v>10.12842</v>
-      </c>
-      <c r="AA21">
-        <v>4658.0529999999999</v>
-      </c>
-      <c r="AB21" s="3">
-        <v>9.495199E-2</v>
-      </c>
-      <c r="AC21">
-        <v>0.26241229999999999</v>
-      </c>
-      <c r="AD21">
-        <v>0.2</v>
-      </c>
-      <c r="AE21">
-        <v>0.2</v>
-      </c>
-      <c r="AF21">
-        <v>136.4796</v>
-      </c>
-      <c r="AG21">
-        <v>129.1413</v>
-      </c>
-      <c r="AH21">
-        <v>144.23500000000001</v>
-      </c>
-      <c r="AI21" s="3">
-        <v>2.812332E-2</v>
-      </c>
-      <c r="AJ21">
-        <v>0.34752929999999999</v>
-      </c>
-      <c r="AK21">
-        <v>0.29697499999999999</v>
-      </c>
-      <c r="AL21">
-        <v>0.40668959999999998</v>
-      </c>
-      <c r="AM21" s="3">
-        <v>8.0036189999999993E-2</v>
-      </c>
-      <c r="AN21" s="3">
-        <v>7.450677E-2</v>
-      </c>
-      <c r="AO21" s="3">
-        <v>6.6714209999999996E-2</v>
-      </c>
-      <c r="AP21" s="3">
-        <v>8.3209539999999999E-2</v>
-      </c>
-      <c r="AQ21" s="3">
-        <v>5.6246640000000001E-2</v>
-      </c>
-      <c r="AR21">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="22" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22">
-        <v>1</v>
-      </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="S22">
-        <v>1</v>
-      </c>
-      <c r="T22" t="s">
-        <v>34</v>
-      </c>
-      <c r="U22" s="2">
-        <v>43645.697106481479</v>
-      </c>
-      <c r="V22" s="2">
-        <v>43648.642893518518</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
-      </c>
-      <c r="X22">
-        <v>2</v>
-      </c>
-      <c r="Y22">
-        <v>423</v>
-      </c>
-      <c r="Z22">
-        <v>0</v>
-      </c>
-      <c r="AA22">
-        <v>4647.9250000000002</v>
-      </c>
-      <c r="AB22">
-        <v>0.77731799999999995</v>
-      </c>
-      <c r="AC22">
-        <v>0.89421139999999999</v>
-      </c>
-      <c r="AD22">
-        <v>1</v>
-      </c>
-      <c r="AE22">
-        <v>1</v>
-      </c>
-      <c r="AF22">
-        <v>117.9564</v>
-      </c>
-      <c r="AG22">
-        <v>113.51009999999999</v>
-      </c>
-      <c r="AH22">
-        <v>122.57689999999999</v>
-      </c>
-      <c r="AI22" s="3">
-        <v>1.954962E-2</v>
-      </c>
-      <c r="AJ22">
-        <v>0.46524749999999998</v>
-      </c>
-      <c r="AK22">
-        <v>0.40609010000000001</v>
-      </c>
-      <c r="AL22">
-        <v>0.53302269999999996</v>
-      </c>
-      <c r="AM22" s="3">
-        <v>6.9071389999999996E-2</v>
-      </c>
-      <c r="AN22" s="3">
-        <v>5.565486E-2</v>
-      </c>
-      <c r="AO22" s="3">
-        <v>5.1539309999999998E-2</v>
-      </c>
-      <c r="AP22" s="3">
-        <v>6.0099050000000001E-2</v>
-      </c>
-      <c r="AQ22" s="3">
-        <v>3.9099229999999999E-2</v>
-      </c>
-      <c r="AR22">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="23" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="O23">
-        <v>2</v>
-      </c>
-      <c r="P23">
-        <v>3</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="S23">
-        <v>3</v>
-      </c>
-      <c r="T23" t="s">
-        <v>15</v>
-      </c>
-      <c r="U23" s="2">
-        <v>43645.720439814817</v>
-      </c>
-      <c r="V23" s="2">
-        <v>43648.642824074072</v>
-      </c>
-      <c r="W23">
-        <v>3</v>
-      </c>
-      <c r="X23">
-        <v>3</v>
-      </c>
-      <c r="Y23">
-        <v>423</v>
-      </c>
-      <c r="Z23">
-        <v>66.496089999999995</v>
-      </c>
-      <c r="AA23">
-        <v>4714.4210000000003</v>
-      </c>
-      <c r="AB23" s="3">
-        <v>5.9604640000000001E-8</v>
-      </c>
-      <c r="AC23">
-        <v>0</v>
-      </c>
-      <c r="AD23">
-        <v>1E-3</v>
-      </c>
-      <c r="AE23">
-        <v>1E-3</v>
-      </c>
-      <c r="AF23">
-        <v>152.67019999999999</v>
-      </c>
-      <c r="AG23">
-        <v>149.09049999999999</v>
-      </c>
-      <c r="AH23">
-        <v>156.33600000000001</v>
-      </c>
-      <c r="AI23" s="3">
-        <v>1.2071459999999999E-2</v>
-      </c>
-      <c r="AJ23">
-        <v>0.27772720000000001</v>
-      </c>
-      <c r="AK23">
-        <v>0.24579519999999999</v>
-      </c>
-      <c r="AL23">
-        <v>0.31380750000000002</v>
-      </c>
-      <c r="AM23" s="3">
-        <v>6.1846480000000002E-2</v>
-      </c>
-      <c r="AN23" s="3">
-        <v>9.3232809999999999E-2</v>
-      </c>
-      <c r="AO23" s="3">
-        <v>8.8912309999999994E-2</v>
-      </c>
-      <c r="AP23" s="3">
-        <v>9.7763260000000005E-2</v>
-      </c>
-      <c r="AQ23" s="3">
-        <v>2.4142919999999998E-2</v>
-      </c>
-      <c r="AR23">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="24" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="O24">
-        <v>3</v>
-      </c>
-      <c r="P24">
-        <v>2</v>
-      </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24">
-        <v>1</v>
-      </c>
-      <c r="S24">
-        <v>2</v>
-      </c>
-      <c r="T24" t="s">
-        <v>37</v>
-      </c>
-      <c r="U24" s="2">
-        <v>43645.717662037037</v>
-      </c>
-      <c r="V24" s="2">
-        <v>43648.642847222225</v>
-      </c>
-    </row>
-    <row r="26" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="AC26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="AC27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="AC29" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE29" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF29" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG29" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH29" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI29" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ29" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK29" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL29" t="s">
-        <v>23</v>
-      </c>
-      <c r="AM29" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN29" t="s">
-        <v>24</v>
-      </c>
-      <c r="AO29" t="s">
-        <v>25</v>
-      </c>
-      <c r="AP29" t="s">
-        <v>26</v>
-      </c>
-      <c r="AQ29" t="s">
-        <v>50</v>
-      </c>
-      <c r="AR29" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS29" t="s">
-        <v>48</v>
-      </c>
-      <c r="AT29" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU29" t="s">
-        <v>29</v>
-      </c>
-      <c r="AV29" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW29" t="s">
-        <v>55</v>
-      </c>
-      <c r="AX29" t="s">
-        <v>31</v>
-      </c>
-      <c r="AY29" t="s">
-        <v>32</v>
-      </c>
-      <c r="AZ29" t="s">
-        <v>33</v>
-      </c>
-      <c r="BA29" t="s">
-        <v>27</v>
-      </c>
-      <c r="BB29" t="s">
-        <v>51</v>
-      </c>
-      <c r="BC29" t="s">
-        <v>52</v>
-      </c>
-      <c r="BD29" t="s">
-        <v>53</v>
-      </c>
-      <c r="BE29" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="AC30">
-        <v>1</v>
-      </c>
-      <c r="AD30">
-        <v>5</v>
-      </c>
-      <c r="AE30">
-        <v>1</v>
-      </c>
-      <c r="AF30">
-        <v>1</v>
-      </c>
-      <c r="AG30">
-        <v>5</v>
-      </c>
-      <c r="AH30" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI30" s="2">
-        <v>43645.731585648151</v>
-      </c>
-      <c r="AJ30" s="2">
-        <v>43674.886631944442</v>
-      </c>
-      <c r="AK30">
-        <v>5</v>
-      </c>
-      <c r="AL30">
-        <v>2</v>
-      </c>
-      <c r="AM30">
-        <v>217</v>
-      </c>
-      <c r="AN30">
-        <v>0</v>
-      </c>
-      <c r="AO30">
-        <v>2318.1170000000002</v>
-      </c>
-      <c r="AP30">
-        <v>0.14716180000000001</v>
-      </c>
-      <c r="AQ30">
-        <v>0.56517220000000001</v>
-      </c>
-      <c r="AR30">
-        <v>0.7</v>
-      </c>
-      <c r="AS30">
-        <v>0.6</v>
-      </c>
-      <c r="AT30">
-        <v>175.25049999999999</v>
-      </c>
-      <c r="AU30">
-        <v>165.1422</v>
-      </c>
-      <c r="AV30">
-        <v>185.97749999999999</v>
-      </c>
-      <c r="AW30" s="3">
-        <v>3.014762E-2</v>
-      </c>
-      <c r="AX30">
-        <v>0.1081255</v>
-      </c>
-      <c r="AY30" s="3">
-        <v>8.4573930000000005E-2</v>
-      </c>
-      <c r="AZ30">
-        <v>0.13823550000000001</v>
-      </c>
-      <c r="BA30">
-        <v>0.1249208</v>
-      </c>
-      <c r="BB30">
-        <v>0.34132089999999998</v>
-      </c>
-      <c r="BC30">
-        <v>0.30310680000000001</v>
-      </c>
-      <c r="BD30">
-        <v>0.38435269999999999</v>
-      </c>
-      <c r="BE30" s="3">
-        <v>6.029524E-2</v>
-      </c>
-      <c r="BF30">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="31" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="AC31">
-        <v>2</v>
-      </c>
-      <c r="AD31">
-        <v>6</v>
-      </c>
-      <c r="AE31">
-        <v>1</v>
-      </c>
-      <c r="AF31">
-        <v>2</v>
-      </c>
-      <c r="AG31">
-        <v>6</v>
-      </c>
-      <c r="AH31" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI31" s="2">
-        <v>43737.68613425926</v>
-      </c>
-      <c r="AJ31" s="2">
-        <v>43737.703449074077</v>
-      </c>
-      <c r="AK31">
-        <v>6</v>
-      </c>
-      <c r="AL31">
-        <v>2</v>
-      </c>
-      <c r="AM31">
-        <v>210</v>
-      </c>
-      <c r="AN31">
-        <v>0</v>
-      </c>
-      <c r="AO31">
-        <v>540.76480000000004</v>
-      </c>
-      <c r="AP31">
-        <v>0.34628930000000002</v>
-      </c>
-      <c r="AT31">
-        <v>160.1337</v>
-      </c>
-      <c r="AU31">
-        <v>147.2749</v>
-      </c>
-      <c r="AV31">
-        <v>174.11519999999999</v>
-      </c>
-      <c r="AW31" s="3">
-        <v>4.2479589999999998E-2</v>
-      </c>
-      <c r="AX31">
-        <v>0.12532579999999999</v>
-      </c>
-      <c r="AY31" s="3">
-        <v>9.571064E-2</v>
-      </c>
-      <c r="AZ31">
-        <v>0.16410459999999999</v>
-      </c>
-      <c r="BA31">
-        <v>0.13745579999999999</v>
-      </c>
-      <c r="BB31">
-        <v>0.44518770000000002</v>
-      </c>
-      <c r="BC31">
-        <v>0.37664589999999998</v>
-      </c>
-      <c r="BD31">
-        <v>0.52620259999999996</v>
-      </c>
-      <c r="BE31" s="3">
-        <v>8.4959190000000004E-2</v>
-      </c>
-      <c r="BF31">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="32" spans="15:58" x14ac:dyDescent="0.3">
-      <c r="AC32">
-        <v>2</v>
-      </c>
-      <c r="AD32">
-        <v>4</v>
-      </c>
-      <c r="AE32">
-        <v>1</v>
-      </c>
-      <c r="AF32">
-        <v>1</v>
-      </c>
-      <c r="AG32">
-        <v>4</v>
-      </c>
-      <c r="AH32" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI32" s="2">
-        <v>43645.728414351855</v>
-      </c>
-      <c r="AJ32" s="2">
-        <v>43674.88685185185</v>
-      </c>
-      <c r="AK32">
-        <v>4</v>
-      </c>
-      <c r="AL32">
-        <v>2</v>
-      </c>
-      <c r="AM32">
-        <v>217</v>
-      </c>
-      <c r="AN32">
-        <v>0</v>
-      </c>
-      <c r="AO32">
-        <v>2318.1170000000002</v>
-      </c>
-      <c r="AP32">
-        <v>0.14716180000000001</v>
-      </c>
-      <c r="AQ32">
-        <v>0.56517220000000001</v>
-      </c>
-      <c r="AR32">
-        <v>0.7</v>
-      </c>
-      <c r="AS32">
-        <v>0.6</v>
-      </c>
-      <c r="AT32">
-        <v>175.25049999999999</v>
-      </c>
-      <c r="AU32">
-        <v>165.1422</v>
-      </c>
-      <c r="AV32">
-        <v>185.97749999999999</v>
-      </c>
-      <c r="AW32" s="3">
-        <v>3.014762E-2</v>
-      </c>
-      <c r="AX32">
-        <v>0.1081255</v>
-      </c>
-      <c r="AY32" s="3">
-        <v>8.4573930000000005E-2</v>
-      </c>
-      <c r="AZ32">
-        <v>0.13823550000000001</v>
-      </c>
-      <c r="BA32">
-        <v>0.1249208</v>
-      </c>
-      <c r="BB32">
-        <v>0.34132089999999998</v>
-      </c>
-      <c r="BC32">
-        <v>0.30310680000000001</v>
-      </c>
-      <c r="BD32">
-        <v>0.38435269999999999</v>
-      </c>
-      <c r="BE32" s="3">
-        <v>6.029524E-2</v>
-      </c>
-      <c r="BF32">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="29:58" x14ac:dyDescent="0.3">
-      <c r="AC33">
-        <v>2</v>
-      </c>
-      <c r="AD33">
-        <v>3</v>
-      </c>
-      <c r="AE33">
-        <v>1</v>
-      </c>
-      <c r="AF33">
-        <v>1</v>
-      </c>
-      <c r="AG33">
-        <v>3</v>
-      </c>
-      <c r="AH33" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI33" s="2">
-        <v>43645.720439814817</v>
-      </c>
-      <c r="AJ33" s="2">
-        <v>43674.886793981481</v>
-      </c>
-      <c r="AK33">
-        <v>3</v>
-      </c>
-      <c r="AL33">
-        <v>3</v>
-      </c>
-      <c r="AM33">
-        <v>217</v>
-      </c>
-      <c r="AN33">
-        <v>1.529053</v>
-      </c>
-      <c r="AO33">
-        <v>2319.6460000000002</v>
-      </c>
-      <c r="AP33">
-        <v>0.10358630000000001</v>
-      </c>
-      <c r="AQ33">
-        <v>0.14296420000000001</v>
-      </c>
-      <c r="AR33">
-        <v>0.3</v>
-      </c>
-      <c r="AS33">
-        <v>0.2</v>
-      </c>
-      <c r="AT33">
-        <v>162.1482</v>
-      </c>
-      <c r="AU33">
-        <v>133.05889999999999</v>
-      </c>
-      <c r="AV33">
-        <v>197.59710000000001</v>
-      </c>
-      <c r="AW33">
-        <v>0.10056130000000001</v>
-      </c>
-      <c r="AX33">
-        <v>0.12630540000000001</v>
-      </c>
-      <c r="AY33" s="3">
-        <v>8.0956379999999994E-2</v>
-      </c>
-      <c r="AZ33">
-        <v>0.1970576</v>
-      </c>
-      <c r="BA33">
-        <v>0.22895399999999999</v>
-      </c>
-      <c r="BB33">
-        <v>0.29219230000000002</v>
-      </c>
-      <c r="BC33">
-        <v>0.1973346</v>
-      </c>
-      <c r="BD33">
-        <v>0.43264770000000002</v>
-      </c>
-      <c r="BE33">
-        <v>0.20112250000000001</v>
-      </c>
-      <c r="BF33">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="34" spans="29:58" x14ac:dyDescent="0.3">
-      <c r="AC34">
-        <v>2</v>
-      </c>
-      <c r="AD34">
-        <v>2</v>
-      </c>
-      <c r="AE34">
-        <v>1</v>
-      </c>
-      <c r="AF34">
-        <v>1</v>
-      </c>
-      <c r="AG34">
-        <v>2</v>
-      </c>
-      <c r="AH34" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI34" s="2">
-        <v>43645.717662037037</v>
-      </c>
-      <c r="AJ34" s="2">
-        <v>43674.886747685188</v>
-      </c>
-      <c r="AK34">
-        <v>2</v>
-      </c>
-      <c r="AL34">
-        <v>2</v>
-      </c>
-      <c r="AM34">
-        <v>217</v>
-      </c>
-      <c r="AN34" s="3">
-        <v>7.0800780000000001E-3</v>
-      </c>
-      <c r="AO34">
-        <v>2318.1239999999998</v>
-      </c>
-      <c r="AP34" s="3">
-        <v>2.5541129999999999E-2</v>
-      </c>
-      <c r="AQ34">
-        <v>0.18720819999999999</v>
-      </c>
-      <c r="AR34">
-        <v>0.2</v>
-      </c>
-      <c r="AS34">
-        <v>0.15</v>
-      </c>
-      <c r="AT34">
-        <v>159.59049999999999</v>
-      </c>
-      <c r="AU34">
-        <v>153.6918</v>
-      </c>
-      <c r="AV34">
-        <v>165.71559999999999</v>
-      </c>
-      <c r="AW34" s="3">
-        <v>1.9109250000000001E-2</v>
-      </c>
-      <c r="AX34">
-        <v>0.13038649999999999</v>
-      </c>
-      <c r="AY34">
-        <v>0.10374890000000001</v>
-      </c>
-      <c r="AZ34">
-        <v>0.16386329999999999</v>
-      </c>
-      <c r="BA34">
-        <v>0.1158893</v>
-      </c>
-      <c r="BB34">
-        <v>0.28304689999999999</v>
-      </c>
-      <c r="BC34">
-        <v>0.2625152</v>
-      </c>
-      <c r="BD34">
-        <v>0.30518430000000002</v>
-      </c>
-      <c r="BE34" s="3">
-        <v>3.8218509999999997E-2</v>
-      </c>
-      <c r="BF34">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="35" spans="29:58" x14ac:dyDescent="0.3">
-      <c r="AC35">
-        <v>2</v>
-      </c>
-      <c r="AD35">
-        <v>1</v>
-      </c>
-      <c r="AE35">
-        <v>1</v>
-      </c>
-      <c r="AF35">
-        <v>1</v>
-      </c>
-      <c r="AG35">
-        <v>1</v>
-      </c>
-      <c r="AH35" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI35" s="2">
-        <v>43645.697106481479</v>
-      </c>
-      <c r="AJ35" s="2">
-        <v>43674.886701388888</v>
-      </c>
-      <c r="AK35">
-        <v>1</v>
-      </c>
-      <c r="AL35">
-        <v>3</v>
-      </c>
-      <c r="AM35">
-        <v>217</v>
-      </c>
-      <c r="AN35">
-        <v>0.60498050000000003</v>
-      </c>
-      <c r="AO35">
-        <v>2318.7220000000002</v>
-      </c>
-      <c r="AP35">
-        <v>0.1377823</v>
-      </c>
-      <c r="AQ35">
-        <v>0.37579010000000002</v>
-      </c>
-      <c r="AR35">
-        <v>0.6</v>
-      </c>
-      <c r="AS35">
-        <v>0.4</v>
-      </c>
-      <c r="AT35">
-        <v>170.42619999999999</v>
-      </c>
-      <c r="AU35">
-        <v>114.8938</v>
-      </c>
-      <c r="AV35">
-        <v>252.79939999999999</v>
-      </c>
-      <c r="AW35">
-        <v>0.20205419999999999</v>
-      </c>
-      <c r="AX35">
-        <v>0.11433359999999999</v>
-      </c>
-      <c r="AY35" s="3">
-        <v>5.1807619999999999E-2</v>
-      </c>
-      <c r="AZ35">
-        <v>0.25232149999999998</v>
-      </c>
-      <c r="BA35">
-        <v>0.41865659999999999</v>
-      </c>
-      <c r="BB35">
-        <v>0.32278760000000001</v>
-      </c>
-      <c r="BC35">
-        <v>0.14996119999999999</v>
-      </c>
-      <c r="BD35">
-        <v>0.69479199999999997</v>
-      </c>
-      <c r="BE35">
-        <v>0.40410849999999998</v>
-      </c>
-      <c r="BF35">
-        <v>214</v>
-      </c>
+    <row r="12" spans="7:81" x14ac:dyDescent="0.3">
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="BD12" s="3"/>
+    </row>
+    <row r="19" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="AI19" s="3"/>
+      <c r="AM19" s="3"/>
+      <c r="AQ19" s="3"/>
+    </row>
+    <row r="20" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="AB20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AM20" s="3"/>
+      <c r="AN20" s="3"/>
+      <c r="AO20" s="3"/>
+      <c r="AP20" s="3"/>
+      <c r="AQ20" s="3"/>
+    </row>
+    <row r="21" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="AB21" s="3"/>
+      <c r="AI21" s="3"/>
+      <c r="AM21" s="3"/>
+      <c r="AN21" s="3"/>
+      <c r="AO21" s="3"/>
+      <c r="AP21" s="3"/>
+      <c r="AQ21" s="3"/>
+    </row>
+    <row r="22" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="AI22" s="3"/>
+      <c r="AM22" s="3"/>
+      <c r="AN22" s="3"/>
+      <c r="AO22" s="3"/>
+      <c r="AP22" s="3"/>
+      <c r="AQ22" s="3"/>
+    </row>
+    <row r="23" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="AB23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+    </row>
+    <row r="24" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+    </row>
+    <row r="30" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="AI30" s="2"/>
+      <c r="AJ30" s="2"/>
+      <c r="AW30" s="3"/>
+      <c r="AY30" s="3"/>
+      <c r="BE30" s="3"/>
+    </row>
+    <row r="31" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="AI31" s="2"/>
+      <c r="AJ31" s="2"/>
+      <c r="AW31" s="3"/>
+      <c r="AY31" s="3"/>
+      <c r="BE31" s="3"/>
+    </row>
+    <row r="32" spans="21:57" x14ac:dyDescent="0.3">
+      <c r="AI32" s="2"/>
+      <c r="AJ32" s="2"/>
+      <c r="AW32" s="3"/>
+      <c r="AY32" s="3"/>
+      <c r="BE32" s="3"/>
+    </row>
+    <row r="33" spans="35:57" x14ac:dyDescent="0.3">
+      <c r="AI33" s="2"/>
+      <c r="AJ33" s="2"/>
+      <c r="AY33" s="3"/>
+    </row>
+    <row r="34" spans="35:57" x14ac:dyDescent="0.3">
+      <c r="AI34" s="2"/>
+      <c r="AJ34" s="2"/>
+      <c r="AN34" s="3"/>
+      <c r="AP34" s="3"/>
+      <c r="AW34" s="3"/>
+      <c r="BE34" s="3"/>
+    </row>
+    <row r="35" spans="35:57" x14ac:dyDescent="0.3">
+      <c r="AI35" s="2"/>
+      <c r="AJ35" s="2"/>
+      <c r="AY35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AutoDS Cosmétique rapport pour démo équipe noyau DS (samples 3 et 4)
</commit_message>
<xml_diff>
--- a/AutoDS/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
+++ b/AutoDS/refout/ACDC2019-Papyrus-ALAARV-TURMER-resultats-distance-73.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\jpm-sandbox\perso\AutoDS\refout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6064B84-941B-4C26-9DB1-4298CCE740CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A4CAF4-FE04-412B-A5BA-52EB3385AE11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="48" windowWidth="19620" windowHeight="9564" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="96" yWindow="48" windowWidth="19620" windowHeight="9564" tabRatio="272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultats" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="68">
   <si>
     <t>TURMER</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>Hazard Cos TGD FitCls</t>
+  </si>
+  <si>
+    <t>Prec.</t>
+  </si>
+  <si>
+    <t>1 déc.</t>
+  </si>
+  <si>
+    <t>6 déc.</t>
   </si>
 </sst>
 </file>
@@ -653,13 +662,13 @@
   <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" customWidth="1"/>
     <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
@@ -691,7 +700,7 @@
         <v>40</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>33</v>
@@ -789,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>35</v>
@@ -876,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>35</v>
@@ -963,7 +972,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>35</v>
@@ -1050,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>35</v>
@@ -1137,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>35</v>
@@ -1160,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>36</v>
@@ -1247,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>36</v>
@@ -1334,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>36</v>
@@ -1421,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>36</v>
@@ -1511,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>36</v>
@@ -1598,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>36</v>
@@ -1621,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>36</v>
@@ -1708,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>36</v>
@@ -1795,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>36</v>
@@ -1882,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>36</v>
@@ -1977,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>36</v>
@@ -2064,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>36</v>
@@ -2087,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>36</v>
@@ -2174,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>36</v>
@@ -2261,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>36</v>
@@ -2353,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>36</v>
@@ -2444,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>36</v>
@@ -2531,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>36</v>
@@ -2618,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>36</v>
@@ -2705,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>36</v>
@@ -2792,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>36</v>
@@ -2889,7 +2898,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>36</v>
@@ -2976,7 +2985,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>36</v>
@@ -3072,7 +3081,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>36</v>
@@ -3159,7 +3168,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>36</v>
@@ -3246,7 +3255,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>36</v>
@@ -3333,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>36</v>

</xml_diff>